<commit_message>
work all over the place mainly of affinity section
git-svn-id: file://localhost/tmp/svn2git/svn@7688 defb5e50-622e-49ec-a68e-d72c7db87b45
</commit_message>
<xml_diff>
--- a/papers/ccpe-cloud12/performance/pd.xlsx
+++ b/papers/ccpe-cloud12/performance/pd.xlsx
@@ -10,12 +10,13 @@
     <sheet name="Blatt1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Blatt1!$A$1:$L$32</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Blatt1!$A$1:$L$31</definedName>
     <definedName name="pd" localSheetId="0">Blatt1!$A$1:$J$31</definedName>
+    <definedName name="pd_random" localSheetId="0">Blatt1!$A$32:$J$45</definedName>
   </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <pivotCaches>
-    <pivotCache cacheId="7" r:id="rId2"/>
+    <pivotCache cacheId="9" r:id="rId2"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -27,8 +28,24 @@
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" name="pd.csv" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" codePage="10000" sourceFile="Macintosh HD:Users:luckow:Dropbox:SAGA:papers:ccpe-cloud12:performance:pd.csv" comma="1" qualifier="none">
+  <connection id="1" name="pd_random.csv" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" sourceFile="Macintosh HD:Users:luckow:Dropbox:SAGA:papers:ccpe-cloud12:performance:pd_random.csv" comma="1">
+      <textFields count="10">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="2" name="pd.csv" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" sourceFile="Macintosh HD:Users:luckow:Dropbox:SAGA:papers:ccpe-cloud12:performance:pd.csv" comma="1" qualifier="none">
       <textFields count="10">
         <textField/>
         <textField/>
@@ -47,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="36">
   <si>
     <t>Run</t>
   </si>
@@ -136,13 +153,25 @@
     <t>Upload</t>
   </si>
   <si>
-    <t>Pilot Queue Time</t>
+    <t>Download</t>
   </si>
   <si>
-    <t xml:space="preserve">CU Runtime </t>
+    <t>s3://pilot-data-e80f3c86-f53f-11e1-999d-00215ec9e3ac</t>
   </si>
   <si>
-    <t>Download</t>
+    <t>gs://pilot-data-68009520-f5ef-11e1-922b-00215ec9e3ac</t>
+  </si>
+  <si>
+    <t>gs://pilot-data-03420b66-f601-11e1-a1b1-00215ec9e3ac</t>
+  </si>
+  <si>
+    <t>/dev/urandom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pilot Queue </t>
+  </si>
+  <si>
+    <t xml:space="preserve">CU Compute </t>
   </si>
 </sst>
 </file>
@@ -150,7 +179,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -211,8 +240,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
@@ -224,64 +255,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="5">
     <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="16">
+  <dxfs count="3">
     <dxf>
-      <numFmt numFmtId="168" formatCode="0.0"/>
+      <numFmt numFmtId="164" formatCode="0.0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="168" formatCode="0.0"/>
+      <numFmt numFmtId="164" formatCode="0.0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="168" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="0.0"/>
+      <numFmt numFmtId="164" formatCode="0.0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -326,8 +320,8 @@
           <c:spPr>
             <a:solidFill>
               <a:schemeClr val="tx1">
-                <a:lumMod val="75000"/>
-                <a:lumOff val="25000"/>
+                <a:lumMod val="85000"/>
+                <a:lumOff val="15000"/>
               </a:schemeClr>
             </a:solidFill>
           </c:spPr>
@@ -353,10 +347,10 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>216.4387627840833</c:v>
+                  <c:v>220.7107000827</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1099.532858477333</c:v>
+                  <c:v>791.47931707025</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -376,6 +370,14 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="65000"/>
+                <a:lumOff val="35000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
@@ -398,10 +400,10 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>113.9241666992417</c:v>
+                  <c:v>110.47700002196</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>66.96222223176667</c:v>
+                  <c:v>139.105000019025</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -416,11 +418,18 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Pilot Queue Time</c:v>
+                  <c:v>Pilot Queue </c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="bg1">
+                <a:lumMod val="65000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:errBars>
             <c:errBarType val="both"/>
@@ -433,10 +442,10 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="2"/>
                   <c:pt idx="0">
-                    <c:v>152.7666197820535</c:v>
+                    <c:v>211.5752818356191</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>588.4114821609811</c:v>
+                    <c:v>836.5967639974622</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -448,10 +457,10 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="2"/>
                   <c:pt idx="0">
-                    <c:v>152.7666197820535</c:v>
+                    <c:v>211.5752818356191</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>588.4114821609811</c:v>
+                    <c:v>836.5967639974622</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -487,10 +496,10 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>74.32076829672501</c:v>
+                  <c:v>74.09683890343001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>36.09490707184445</c:v>
+                  <c:v>32.68710553645</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -505,11 +514,18 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>CU Runtime </c:v>
+                  <c:v>CU Compute </c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="bg1">
+                <a:lumMod val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
@@ -532,10 +548,10 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>5.510833323003333</c:v>
+                  <c:v>3.2009999990462</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.951111104753666</c:v>
+                  <c:v>2.1349999904625</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -551,11 +567,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="-2117269784"/>
-        <c:axId val="-2117816136"/>
+        <c:axId val="2093810536"/>
+        <c:axId val="2093813176"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2117269784"/>
+        <c:axId val="2093810536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -574,7 +590,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2117816136"/>
+        <c:crossAx val="2093813176"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -582,7 +598,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2117816136"/>
+        <c:axId val="2093813176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -600,7 +616,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="de-DE" sz="2800"/>
-                  <a:t>Runtime (in sec)</a:t>
+                  <a:t>Time (in sec)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -622,7 +638,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2117269784"/>
+        <c:crossAx val="2093810536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -671,7 +687,7 @@
     <xdr:to>
       <xdr:col>21</xdr:col>
       <xdr:colOff>622300</xdr:colOff>
-      <xdr:row>68</xdr:row>
+      <xdr:row>62</xdr:row>
       <xdr:rowOff>127000</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -695,19 +711,18 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Andre Luckow" refreshedDate="41154.493903703704" createdVersion="4" refreshedVersion="4" minRefreshableVersion="3" recordCount="30">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Andre Luckow" refreshedDate="41156.362004629627" createdVersion="4" refreshedVersion="4" minRefreshableVersion="3" recordCount="44">
   <cacheSource type="worksheet">
-    <worksheetSource ref="A1:J31" sheet="Blatt1"/>
+    <worksheetSource ref="A1:L45" sheet="Blatt1"/>
   </cacheSource>
-  <cacheFields count="10">
+  <cacheFields count="12">
     <cacheField name="Run" numFmtId="0">
       <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="0" maxValue="9"/>
     </cacheField>
     <cacheField name="PC" numFmtId="0">
-      <sharedItems count="3">
+      <sharedItems count="2">
         <s v="ec2+ssh://aws.amazon.com/"/>
         <s v="gce+ssh://google.com"/>
-        <s v="euca+ssh://149.165.146.135:8773/services/Eucalyptus" u="1"/>
       </sharedItems>
     </cacheField>
     <cacheField name="PD" numFmtId="0">
@@ -722,20 +737,29 @@
         <n v="128"/>
       </sharedItems>
     </cacheField>
-    <cacheField name="Upload Time" numFmtId="168">
+    <cacheField name="Upload Time" numFmtId="0">
       <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="17.992821216599999" maxValue="2002.243119"/>
     </cacheField>
-    <cacheField name="Pilot Queue" numFmtId="168">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="32.472221851299999" maxValue="94.932879924800005"/>
+    <cacheField name="Pilot Queue" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="29.4648599625" maxValue="94.932879924800005"/>
     </cacheField>
-    <cacheField name="Total Runtime" numFmtId="168">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="99.422956943499997" maxValue="2154.2311692200001"/>
+    <cacheField name="Total Runtime" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="99.422956943499997" maxValue="2211.25476789"/>
     </cacheField>
-    <cacheField name="CU qtime" numFmtId="168">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="9.4400000572200007" maxValue="197.910000086"/>
+    <cacheField name="CU qtime" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="9.4400000572200007" maxValue="455.17000007600001"/>
     </cacheField>
-    <cacheField name="CU Runtime" numFmtId="168">
+    <cacheField name="CU Runtime" numFmtId="0">
       <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="-1" maxValue="11.7300000191"/>
+    </cacheField>
+    <cacheField name="Delta Runtime" numFmtId="164">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="7.1093659396300382" maxValue="37.796485900610037"/>
+    </cacheField>
+    <cacheField name="Remark" numFmtId="0">
+      <sharedItems count="2">
+        <s v="/dev/zero"/>
+        <s v="/dev/urandom"/>
+      </sharedItems>
     </cacheField>
   </cacheFields>
   <extLst>
@@ -747,7 +771,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="30">
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="44">
   <r>
     <n v="0"/>
     <x v="0"/>
@@ -759,6 +783,8 @@
     <n v="366.30230307599999"/>
     <n v="116.230000019"/>
     <n v="4.4500000476799997"/>
+    <n v="14.560280084419958"/>
+    <x v="0"/>
   </r>
   <r>
     <n v="0"/>
@@ -771,6 +797,8 @@
     <n v="845.18161511400001"/>
     <n v="120.150000095"/>
     <n v="5.1199998855600004"/>
+    <n v="7.9353032114399866"/>
+    <x v="0"/>
   </r>
   <r>
     <n v="0"/>
@@ -783,6 +811,8 @@
     <n v="117.367043972"/>
     <n v="13.599999904600001"/>
     <n v="4.17000007629"/>
+    <n v="13.367931842810009"/>
+    <x v="0"/>
   </r>
   <r>
     <n v="0"/>
@@ -795,6 +825,8 @@
     <n v="120.786075115"/>
     <n v="15.2100000381"/>
     <n v="4.1400001049000004"/>
+    <n v="7.8964829443000042"/>
+    <x v="0"/>
   </r>
   <r>
     <n v="0"/>
@@ -807,6 +839,8 @@
     <n v="121.42557096500001"/>
     <n v="17.7699999809"/>
     <n v="1.1800000667599999"/>
+    <n v="8.2398309710400071"/>
+    <x v="0"/>
   </r>
   <r>
     <n v="0"/>
@@ -819,6 +853,8 @@
     <n v="180.41024804099999"/>
     <n v="9.4400000572200007"/>
     <n v="1.09999990463"/>
+    <n v="8.6135549540499596"/>
+    <x v="0"/>
   </r>
   <r>
     <n v="1"/>
@@ -831,6 +867,8 @@
     <n v="122.424413919"/>
     <n v="13.5399999619"/>
     <n v="-1"/>
+    <n v="12.644558906100002"/>
+    <x v="0"/>
   </r>
   <r>
     <n v="1"/>
@@ -843,6 +881,8 @@
     <n v="159.18596100799999"/>
     <n v="16.4100000858"/>
     <n v="4.5699999332400001"/>
+    <n v="8.2077400683599819"/>
+    <x v="0"/>
   </r>
   <r>
     <n v="2"/>
@@ -855,6 +895,8 @@
     <n v="99.422956943499997"/>
     <n v="16.650000095399999"/>
     <n v="5.1299998760200003"/>
+    <n v="13.430824041380006"/>
+    <x v="0"/>
   </r>
   <r>
     <n v="2"/>
@@ -867,6 +909,8 @@
     <n v="156.98407197"/>
     <n v="17.849999904600001"/>
     <n v="3.09000015259"/>
+    <n v="8.253701925309997"/>
+    <x v="0"/>
   </r>
   <r>
     <n v="3"/>
@@ -879,6 +923,8 @@
     <n v="130.146358013"/>
     <n v="11.8100001812"/>
     <n v="1.1699998378800001"/>
+    <n v="8.1793749331200019"/>
+    <x v="0"/>
   </r>
   <r>
     <n v="0"/>
@@ -891,6 +937,8 @@
     <n v="334.128916979"/>
     <n v="100.49000001"/>
     <n v="5.92000007629"/>
+    <n v="13.109730719809988"/>
+    <x v="0"/>
   </r>
   <r>
     <n v="0"/>
@@ -903,6 +951,8 @@
     <n v="1976.1700248699999"/>
     <n v="69.259999990500006"/>
     <n v="3.9700000286099999"/>
+    <n v="8.1437099005897835"/>
+    <x v="0"/>
   </r>
   <r>
     <n v="1"/>
@@ -915,6 +965,8 @@
     <n v="388.31233096099999"/>
     <n v="103.910000086"/>
     <n v="5.1999998092700004"/>
+    <n v="8.4392030238299753"/>
+    <x v="0"/>
   </r>
   <r>
     <n v="1"/>
@@ -927,6 +979,8 @@
     <n v="816.00404596299995"/>
     <n v="80.5"/>
     <n v="1.61000013351"/>
+    <n v="7.3199648849899859"/>
+    <x v="0"/>
   </r>
   <r>
     <n v="2"/>
@@ -939,6 +993,8 @@
     <n v="607.498153925"/>
     <n v="197.910000086"/>
     <n v="2.8399999141699999"/>
+    <n v="7.1093659396300382"/>
+    <x v="0"/>
   </r>
   <r>
     <n v="2"/>
@@ -951,6 +1007,8 @@
     <n v="1842.7665791500001"/>
     <n v="51.3399999142"/>
     <n v="3.2999999523199999"/>
+    <n v="8.6895410985800936"/>
+    <x v="0"/>
   </r>
   <r>
     <n v="3"/>
@@ -963,6 +1021,8 @@
     <n v="374.15741992"/>
     <n v="110.230000019"/>
     <n v="11.7300000191"/>
+    <n v="7.6052060126000356"/>
+    <x v="0"/>
   </r>
   <r>
     <n v="3"/>
@@ -975,6 +1035,8 @@
     <n v="815.74461007100001"/>
     <n v="52.799999952299999"/>
     <n v="3.9300000667599999"/>
+    <n v="8.6064710611399278"/>
+    <x v="0"/>
   </r>
   <r>
     <n v="4"/>
@@ -987,6 +1049,8 @@
     <n v="329.81398510899999"/>
     <n v="105.130000114"/>
     <n v="5.7599999904599999"/>
+    <n v="14.680315971239963"/>
+    <x v="0"/>
   </r>
   <r>
     <n v="4"/>
@@ -999,6 +1063,8 @@
     <n v="809.29317307500003"/>
     <n v="51.090000152599998"/>
     <n v="1.84999990463"/>
+    <n v="8.3644220831702114"/>
+    <x v="0"/>
   </r>
   <r>
     <n v="5"/>
@@ -1011,6 +1077,8 @@
     <n v="362.74508500100001"/>
     <n v="97.380000114400005"/>
     <n v="6.7599999904599999"/>
+    <n v="7.3524658679399977"/>
+    <x v="0"/>
   </r>
   <r>
     <n v="5"/>
@@ -1023,6 +1091,8 @@
     <n v="2154.2311692200001"/>
     <n v="100.359999895"/>
     <n v="3.9900000095400001"/>
+    <n v="7.1515111900603188"/>
+    <x v="0"/>
   </r>
   <r>
     <n v="6"/>
@@ -1035,6 +1105,8 @@
     <n v="356.379965067"/>
     <n v="98.759999990500006"/>
     <n v="5.1900000572199998"/>
+    <n v="7.5511209967799573"/>
+    <x v="0"/>
   </r>
   <r>
     <n v="6"/>
@@ -1047,6 +1119,8 @@
     <n v="817.61335206000001"/>
     <n v="56.420000076299999"/>
     <n v="4.0599999427800002"/>
+    <n v="8.8604111671199917"/>
+    <x v="0"/>
   </r>
   <r>
     <n v="7"/>
@@ -1059,6 +1133,8 @@
     <n v="339.21266293500003"/>
     <n v="110.730000019"/>
     <n v="5.8199999332400001"/>
+    <n v="15.025970935559997"/>
+    <x v="0"/>
   </r>
   <r>
     <n v="7"/>
@@ -1071,6 +1147,8 @@
     <n v="855.21460199399996"/>
     <n v="56.350000143099997"/>
     <n v="0.78999996185300003"/>
+    <n v="8.1836228370469826"/>
+    <x v="0"/>
   </r>
   <r>
     <n v="8"/>
@@ -1083,6 +1161,8 @@
     <n v="378.10926198999999"/>
     <n v="102.25"/>
     <n v="1.84000015259"/>
+    <n v="7.4114298826100367"/>
+    <x v="0"/>
   </r>
   <r>
     <n v="8"/>
@@ -1095,6 +1175,8 @@
     <n v="835.98509693100004"/>
     <n v="84.539999961899994"/>
     <n v="3.0599999427800002"/>
+    <n v="7.8331091400200421"/>
+    <x v="0"/>
   </r>
   <r>
     <n v="9"/>
@@ -1107,19 +1189,216 @@
     <n v="359.37256908400002"/>
     <n v="103.919999838"/>
     <n v="5.5"/>
+    <n v="8.0995032785000376"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="0"/>
+    <x v="0"/>
+    <s v="s3://pilot-data-e80f3c86-f53f-11e1-999d-00215ec9e3ac"/>
+    <n v="1"/>
+    <x v="0"/>
+    <n v="153.41368102999999"/>
+    <n v="43.968811988799999"/>
+    <n v="266.67451405499997"/>
+    <n v="57.149999856900003"/>
+    <n v="3.2900002002700002"/>
+    <n v="8.8520209790299873"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="1"/>
+    <x v="0"/>
+    <s v="s3://pilot-data-e80f3c86-f53f-11e1-999d-00215ec9e3ac"/>
+    <n v="1"/>
+    <x v="0"/>
+    <n v="167.724998951"/>
+    <n v="76.002597093600002"/>
+    <n v="301.00753998800002"/>
+    <n v="45.920000076299999"/>
+    <n v="2.9800000190699998"/>
+    <n v="8.3799438480299955"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="2"/>
+    <x v="0"/>
+    <s v="s3://pilot-data-e80f3c86-f53f-11e1-999d-00215ec9e3ac"/>
+    <n v="1"/>
+    <x v="0"/>
+    <n v="155.02358794200001"/>
+    <n v="50.976006030999997"/>
+    <n v="279.27387380599998"/>
+    <n v="55.349999904599997"/>
+    <n v="4.4600000381499996"/>
+    <n v="13.464279890249998"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="3"/>
+    <x v="0"/>
+    <s v="s3://pilot-data-e80f3c86-f53f-11e1-999d-00215ec9e3ac"/>
+    <n v="1"/>
+    <x v="0"/>
+    <n v="175.75231814399999"/>
+    <n v="44.699809074400001"/>
+    <n v="317.88112521199997"/>
+    <n v="87.0400002003"/>
+    <n v="1.9199998378800001"/>
+    <n v="8.4689979554199795"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="4"/>
+    <x v="0"/>
+    <s v="s3://pilot-data-e80f3c86-f53f-11e1-999d-00215ec9e3ac"/>
+    <n v="1"/>
+    <x v="0"/>
+    <n v="159.14578890799999"/>
+    <n v="82.960606098200003"/>
+    <n v="371.66165089600003"/>
+    <n v="121.110000134"/>
+    <n v="0.68999981880200001"/>
+    <n v="7.7552559369980258"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="5"/>
+    <x v="0"/>
+    <s v="s3://pilot-data-e80f3c86-f53f-11e1-999d-00215ec9e3ac"/>
+    <n v="1"/>
+    <x v="0"/>
+    <n v="179.50864315000001"/>
+    <n v="82.362717866899999"/>
+    <n v="680.41716098799998"/>
+    <n v="409.81999993300002"/>
+    <n v="1.5300002098100001"/>
+    <n v="7.195799828289978"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="6"/>
+    <x v="0"/>
+    <s v="s3://pilot-data-e80f3c86-f53f-11e1-999d-00215ec9e3ac"/>
+    <n v="1"/>
+    <x v="0"/>
+    <n v="159.794485807"/>
+    <n v="82.955249071099999"/>
+    <n v="362.25430393200003"/>
+    <n v="107.370000124"/>
+    <n v="4.6799998283399997"/>
+    <n v="7.4545691015600255"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="7"/>
+    <x v="0"/>
+    <s v="s3://pilot-data-e80f3c86-f53f-11e1-999d-00215ec9e3ac"/>
+    <n v="1"/>
+    <x v="0"/>
+    <n v="164.00699496300001"/>
+    <n v="94.192369937899997"/>
+    <n v="315.48400592799999"/>
+    <n v="46.210000038099999"/>
+    <n v="2.0699999332400001"/>
+    <n v="9.0046410557599188"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="8"/>
+    <x v="0"/>
+    <s v="s3://pilot-data-e80f3c86-f53f-11e1-999d-00215ec9e3ac"/>
+    <n v="1"/>
+    <x v="0"/>
+    <n v="201.021460056"/>
+    <n v="91.1538639069"/>
+    <n v="359.501757145"/>
+    <n v="53.029999971400002"/>
+    <n v="5.75"/>
+    <n v="8.5464332107000018"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="9"/>
+    <x v="0"/>
+    <s v="s3://pilot-data-e80f3c86-f53f-11e1-999d-00215ec9e3ac"/>
+    <n v="1"/>
+    <x v="0"/>
+    <n v="691.71504187599999"/>
+    <n v="91.696357965499999"/>
+    <n v="916.97918486599997"/>
+    <n v="121.769999981"/>
+    <n v="4.6400001049000004"/>
+    <n v="7.1577849386000025"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="0"/>
+    <x v="1"/>
+    <s v="gs://pilot-data-68009520-f5ef-11e1-922b-00215ec9e3ac"/>
+    <n v="1"/>
+    <x v="0"/>
+    <n v="326.00109910999998"/>
+    <n v="29.4648599625"/>
+    <n v="424.80244493499998"/>
+    <n v="29.759999990499999"/>
+    <n v="1.7799999713900001"/>
+    <n v="37.796485900610037"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="2"/>
+    <x v="1"/>
+    <s v="gs://pilot-data-68009520-f5ef-11e1-922b-00215ec9e3ac"/>
+    <n v="1"/>
+    <x v="0"/>
+    <n v="408.57445120800003"/>
+    <n v="32.547425985300002"/>
+    <n v="480.344675064"/>
+    <n v="22.180000066800002"/>
+    <n v="3.6600000858300001"/>
+    <n v="13.38279771806998"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="5"/>
+    <x v="1"/>
+    <s v="gs://pilot-data-03420b66-f601-11e1-a1b1-00215ec9e3ac"/>
+    <n v="1"/>
+    <x v="0"/>
+    <n v="1708.15698195"/>
+    <n v="35.188234090800002"/>
+    <n v="2211.25476789"/>
+    <n v="455.17000007600001"/>
+    <n v="1.0699999332400001"/>
+    <n v="11.669551839959695"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="6"/>
+    <x v="1"/>
+    <s v="gs://pilot-data-03420b66-f601-11e1-a1b1-00215ec9e3ac"/>
+    <n v="1"/>
+    <x v="0"/>
+    <n v="723.18473601300002"/>
+    <n v="33.547902107200002"/>
+    <n v="819.20431399300003"/>
+    <n v="49.309999942799998"/>
+    <n v="2.0299999713900001"/>
+    <n v="11.131675958610003"/>
+    <x v="1"/>
   </r>
 </pivotCacheRecords>
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0" rowHeaderCaption="">
-  <location ref="O16:U20" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
-  <pivotFields count="10">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="9" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0" rowHeaderCaption="">
+  <location ref="O16:U20" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="2" colPageCount="1"/>
+  <pivotFields count="12">
     <pivotField showAll="0"/>
     <pivotField axis="axisRow" showAll="0">
-      <items count="4">
+      <items count="3">
         <item x="0"/>
-        <item m="1" x="2"/>
         <item x="1"/>
         <item t="default"/>
       </items>
@@ -1134,10 +1413,17 @@
       </items>
     </pivotField>
     <pivotField dataField="1" showAll="0"/>
-    <pivotField dataField="1" numFmtId="168" showAll="0" defaultSubtotal="0"/>
-    <pivotField dataField="1" numFmtId="168" showAll="0" defaultSubtotal="0"/>
+    <pivotField dataField="1" numFmtId="164" showAll="0" defaultSubtotal="0"/>
+    <pivotField dataField="1" numFmtId="164" showAll="0" defaultSubtotal="0"/>
     <pivotField dataField="1" showAll="0"/>
-    <pivotField dataField="1" numFmtId="168" showAll="0" defaultSubtotal="0"/>
+    <pivotField dataField="1" numFmtId="164" showAll="0" defaultSubtotal="0"/>
+    <pivotField numFmtId="164" showAll="0" defaultSubtotal="0"/>
+    <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0" defaultSubtotal="0">
+      <items count="2">
+        <item x="1"/>
+        <item h="1" x="0"/>
+      </items>
+    </pivotField>
   </pivotFields>
   <rowFields count="1">
     <field x="1"/>
@@ -1147,7 +1433,7 @@
       <x/>
     </i>
     <i>
-      <x v="2"/>
+      <x v="1"/>
     </i>
     <i t="grand">
       <x/>
@@ -1176,19 +1462,20 @@
       <x v="5"/>
     </i>
   </colItems>
-  <pageFields count="1">
+  <pageFields count="2">
     <pageField fld="4" hier="-1"/>
+    <pageField fld="11" hier="-1"/>
   </pageFields>
   <dataFields count="6">
     <dataField name="Upload" fld="5" subtotal="average" baseField="0" baseItem="0"/>
     <dataField name="Download" fld="8" subtotal="average" baseField="0" baseItem="0"/>
-    <dataField name="Pilot Queue Time" fld="6" subtotal="average" baseField="0" baseItem="0"/>
+    <dataField name="Pilot Queue " fld="6" subtotal="average" baseField="0" baseItem="0"/>
     <dataField name="Mittelwert - Total Runtime" fld="7" subtotal="average" baseField="0" baseItem="0"/>
-    <dataField name="CU Runtime " fld="9" subtotal="average" baseField="0" baseItem="0"/>
+    <dataField name="CU Compute " fld="9" subtotal="average" baseField="0" baseItem="0"/>
     <dataField name="STABW - Total Runtime" fld="7" subtotal="stdDev" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="1">
-    <format dxfId="15">
+    <format dxfId="2">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
   </formats>
@@ -1202,7 +1489,11 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pd" connectionId="1" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pd_random" connectionId="1" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pd" connectionId="2" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1528,30 +1819,28 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1:U32"/>
+  <dimension ref="A1:W45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="X31" sqref="X31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AB25" sqref="AB25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="8.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="45.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="64.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.1640625" customWidth="1"/>
+    <col min="2" max="2" width="24.6640625" customWidth="1"/>
+    <col min="3" max="3" width="47.6640625" customWidth="1"/>
+    <col min="4" max="4" width="2.1640625" customWidth="1"/>
     <col min="5" max="5" width="5.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19" customWidth="1"/>
-    <col min="7" max="7" width="20.33203125" customWidth="1"/>
-    <col min="8" max="8" width="15.1640625" customWidth="1"/>
+    <col min="6" max="8" width="12.1640625" customWidth="1"/>
     <col min="9" max="10" width="12.1640625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12.1640625" style="8" customWidth="1"/>
     <col min="15" max="15" width="24.6640625" customWidth="1"/>
-    <col min="16" max="16" width="21.83203125" customWidth="1"/>
-    <col min="17" max="17" width="19.1640625" customWidth="1"/>
-    <col min="18" max="18" width="21.1640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.83203125" customWidth="1"/>
+    <col min="17" max="17" width="9.5" customWidth="1"/>
+    <col min="18" max="18" width="11.1640625" customWidth="1"/>
     <col min="19" max="19" width="23" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="21.1640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12" customWidth="1"/>
     <col min="21" max="21" width="20.1640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1664,7 +1953,7 @@
         <v>5.1199998855600004</v>
       </c>
       <c r="K3" s="7">
-        <f t="shared" ref="K3:K31" si="0">H3-(SUM(F3,G3,I3,J3))</f>
+        <f t="shared" ref="K3:K45" si="0">H3-(SUM(F3,G3,I3,J3))</f>
         <v>7.9353032114399866</v>
       </c>
       <c r="L3" t="s">
@@ -2060,6 +2349,12 @@
       <c r="L13" t="s">
         <v>23</v>
       </c>
+      <c r="O13" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="P13" s="4">
+        <v>1024</v>
+      </c>
     </row>
     <row r="14" spans="1:16">
       <c r="A14">
@@ -2100,10 +2395,10 @@
         <v>23</v>
       </c>
       <c r="O14" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="P14" s="4">
-        <v>1024</v>
+        <v>22</v>
+      </c>
+      <c r="P14" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="15" spans="1:16">
@@ -2187,7 +2482,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:21">
+    <row r="17" spans="1:23">
       <c r="A17">
         <v>2</v>
       </c>
@@ -2232,22 +2527,22 @@
         <v>28</v>
       </c>
       <c r="Q17" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="R17" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="S17" t="s">
         <v>24</v>
       </c>
       <c r="T17" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="U17" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="1:21">
+    <row r="18" spans="1:23">
       <c r="A18">
         <v>2</v>
       </c>
@@ -2289,25 +2584,25 @@
         <v>7</v>
       </c>
       <c r="P18" s="5">
-        <v>216.43876278408334</v>
+        <v>220.71070008269999</v>
       </c>
       <c r="Q18" s="5">
-        <v>113.92416669924167</v>
+        <v>110.47700002196</v>
       </c>
       <c r="R18" s="5">
-        <v>74.320768296725007</v>
+        <v>74.096838903430012</v>
       </c>
       <c r="S18" s="5">
-        <v>420.10118909675003</v>
+        <v>417.11351168160002</v>
       </c>
       <c r="T18" s="5">
-        <v>5.5108333230033333</v>
+        <v>3.2009999990461999</v>
       </c>
       <c r="U18" s="5">
-        <v>152.76661978205345</v>
-      </c>
-    </row>
-    <row r="19" spans="1:21">
+        <v>211.57528183561908</v>
+      </c>
+    </row>
+    <row r="19" spans="1:23">
       <c r="A19">
         <v>3</v>
       </c>
@@ -2349,25 +2644,29 @@
         <v>13</v>
       </c>
       <c r="P19" s="5">
-        <v>1099.5328584773333</v>
+        <v>791.47931707024998</v>
       </c>
       <c r="Q19" s="5">
-        <v>66.962222231766674</v>
+        <v>139.105000019025</v>
       </c>
       <c r="R19" s="5">
-        <v>36.094907071844446</v>
+        <v>32.687105536450005</v>
       </c>
       <c r="S19" s="5">
-        <v>1213.6691837037779</v>
+        <v>983.90155047050007</v>
       </c>
       <c r="T19" s="5">
-        <v>2.9511111047536662</v>
+        <v>2.1349999904625001</v>
       </c>
       <c r="U19" s="5">
-        <v>588.41148216098111</v>
-      </c>
-    </row>
-    <row r="20" spans="1:21">
+        <v>836.59676399746229</v>
+      </c>
+      <c r="W19">
+        <f>P19/P18</f>
+        <v>3.5860486907688833</v>
+      </c>
+    </row>
+    <row r="20" spans="1:23">
       <c r="A20">
         <v>3</v>
       </c>
@@ -2409,25 +2708,25 @@
         <v>17</v>
       </c>
       <c r="P20" s="5">
-        <v>594.90766093833338</v>
+        <v>383.7874477934285</v>
       </c>
       <c r="Q20" s="5">
-        <v>93.797619070323819</v>
+        <v>118.65642859255</v>
       </c>
       <c r="R20" s="5">
-        <v>57.93825634320477</v>
+        <v>62.2654865128643</v>
       </c>
       <c r="S20" s="5">
-        <v>760.20175821404769</v>
+        <v>579.05295133557138</v>
       </c>
       <c r="T20" s="5">
-        <v>4.4138095151820469</v>
+        <v>2.896428568022285</v>
       </c>
       <c r="U20" s="5">
-        <v>559.69874661359199</v>
-      </c>
-    </row>
-    <row r="21" spans="1:21">
+        <v>512.94119542916803</v>
+      </c>
+    </row>
+    <row r="21" spans="1:23">
       <c r="A21">
         <v>4</v>
       </c>
@@ -2466,7 +2765,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="22" spans="1:21">
+    <row r="22" spans="1:23">
       <c r="A22">
         <v>4</v>
       </c>
@@ -2505,7 +2804,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="23" spans="1:21">
+    <row r="23" spans="1:23">
       <c r="A23">
         <v>5</v>
       </c>
@@ -2544,7 +2843,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="1:21">
+    <row r="24" spans="1:23">
       <c r="A24">
         <v>5</v>
       </c>
@@ -2583,7 +2882,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:21">
+    <row r="25" spans="1:23">
       <c r="A25">
         <v>6</v>
       </c>
@@ -2622,7 +2921,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:21">
+    <row r="26" spans="1:23">
       <c r="A26">
         <v>6</v>
       </c>
@@ -2661,7 +2960,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="27" spans="1:21">
+    <row r="27" spans="1:23">
       <c r="A27">
         <v>7</v>
       </c>
@@ -2700,7 +2999,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="28" spans="1:21">
+    <row r="28" spans="1:23">
       <c r="A28">
         <v>7</v>
       </c>
@@ -2739,7 +3038,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="29" spans="1:21">
+    <row r="29" spans="1:23">
       <c r="A29">
         <v>8</v>
       </c>
@@ -2778,7 +3077,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="30" spans="1:21">
+    <row r="30" spans="1:23">
       <c r="A30">
         <v>8</v>
       </c>
@@ -2817,7 +3116,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="31" spans="1:21">
+    <row r="31" spans="1:23">
       <c r="A31">
         <v>9</v>
       </c>
@@ -2856,11 +3155,554 @@
         <v>23</v>
       </c>
     </row>
-    <row r="32" spans="1:21" hidden="1">
-      <c r="K32"/>
+    <row r="32" spans="1:23">
+      <c r="A32">
+        <v>0</v>
+      </c>
+      <c r="B32" t="s">
+        <v>7</v>
+      </c>
+      <c r="C32" t="s">
+        <v>30</v>
+      </c>
+      <c r="D32">
+        <v>1</v>
+      </c>
+      <c r="E32">
+        <v>1024</v>
+      </c>
+      <c r="F32">
+        <v>153.41368102999999</v>
+      </c>
+      <c r="G32">
+        <v>43.968811988799999</v>
+      </c>
+      <c r="H32">
+        <v>266.67451405499997</v>
+      </c>
+      <c r="I32">
+        <v>57.149999856900003</v>
+      </c>
+      <c r="J32">
+        <v>3.2900002002700002</v>
+      </c>
+      <c r="K32" s="7">
+        <f t="shared" si="0"/>
+        <v>8.8520209790299873</v>
+      </c>
+      <c r="L32" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12">
+      <c r="A33">
+        <v>1</v>
+      </c>
+      <c r="B33" t="s">
+        <v>7</v>
+      </c>
+      <c r="C33" t="s">
+        <v>30</v>
+      </c>
+      <c r="D33">
+        <v>1</v>
+      </c>
+      <c r="E33">
+        <v>1024</v>
+      </c>
+      <c r="F33">
+        <v>167.724998951</v>
+      </c>
+      <c r="G33">
+        <v>76.002597093600002</v>
+      </c>
+      <c r="H33">
+        <v>301.00753998800002</v>
+      </c>
+      <c r="I33">
+        <v>45.920000076299999</v>
+      </c>
+      <c r="J33">
+        <v>2.9800000190699998</v>
+      </c>
+      <c r="K33" s="7">
+        <f t="shared" si="0"/>
+        <v>8.3799438480299955</v>
+      </c>
+      <c r="L33" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12">
+      <c r="A34">
+        <v>2</v>
+      </c>
+      <c r="B34" t="s">
+        <v>7</v>
+      </c>
+      <c r="C34" t="s">
+        <v>30</v>
+      </c>
+      <c r="D34">
+        <v>1</v>
+      </c>
+      <c r="E34">
+        <v>1024</v>
+      </c>
+      <c r="F34">
+        <v>155.02358794200001</v>
+      </c>
+      <c r="G34">
+        <v>50.976006030999997</v>
+      </c>
+      <c r="H34">
+        <v>279.27387380599998</v>
+      </c>
+      <c r="I34">
+        <v>55.349999904599997</v>
+      </c>
+      <c r="J34">
+        <v>4.4600000381499996</v>
+      </c>
+      <c r="K34" s="7">
+        <f t="shared" si="0"/>
+        <v>13.464279890249998</v>
+      </c>
+      <c r="L34" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12">
+      <c r="A35">
+        <v>3</v>
+      </c>
+      <c r="B35" t="s">
+        <v>7</v>
+      </c>
+      <c r="C35" t="s">
+        <v>30</v>
+      </c>
+      <c r="D35">
+        <v>1</v>
+      </c>
+      <c r="E35">
+        <v>1024</v>
+      </c>
+      <c r="F35">
+        <v>175.75231814399999</v>
+      </c>
+      <c r="G35">
+        <v>44.699809074400001</v>
+      </c>
+      <c r="H35">
+        <v>317.88112521199997</v>
+      </c>
+      <c r="I35">
+        <v>87.0400002003</v>
+      </c>
+      <c r="J35">
+        <v>1.9199998378800001</v>
+      </c>
+      <c r="K35" s="7">
+        <f t="shared" si="0"/>
+        <v>8.4689979554199795</v>
+      </c>
+      <c r="L35" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12">
+      <c r="A36">
+        <v>4</v>
+      </c>
+      <c r="B36" t="s">
+        <v>7</v>
+      </c>
+      <c r="C36" t="s">
+        <v>30</v>
+      </c>
+      <c r="D36">
+        <v>1</v>
+      </c>
+      <c r="E36">
+        <v>1024</v>
+      </c>
+      <c r="F36">
+        <v>159.14578890799999</v>
+      </c>
+      <c r="G36">
+        <v>82.960606098200003</v>
+      </c>
+      <c r="H36">
+        <v>371.66165089600003</v>
+      </c>
+      <c r="I36">
+        <v>121.110000134</v>
+      </c>
+      <c r="J36">
+        <v>0.68999981880200001</v>
+      </c>
+      <c r="K36" s="7">
+        <f t="shared" si="0"/>
+        <v>7.7552559369980258</v>
+      </c>
+      <c r="L36" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12">
+      <c r="A37">
+        <v>5</v>
+      </c>
+      <c r="B37" t="s">
+        <v>7</v>
+      </c>
+      <c r="C37" t="s">
+        <v>30</v>
+      </c>
+      <c r="D37">
+        <v>1</v>
+      </c>
+      <c r="E37">
+        <v>1024</v>
+      </c>
+      <c r="F37">
+        <v>179.50864315000001</v>
+      </c>
+      <c r="G37">
+        <v>82.362717866899999</v>
+      </c>
+      <c r="H37">
+        <v>680.41716098799998</v>
+      </c>
+      <c r="I37">
+        <v>409.81999993300002</v>
+      </c>
+      <c r="J37">
+        <v>1.5300002098100001</v>
+      </c>
+      <c r="K37" s="7">
+        <f t="shared" si="0"/>
+        <v>7.195799828289978</v>
+      </c>
+      <c r="L37" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12">
+      <c r="A38">
+        <v>6</v>
+      </c>
+      <c r="B38" t="s">
+        <v>7</v>
+      </c>
+      <c r="C38" t="s">
+        <v>30</v>
+      </c>
+      <c r="D38">
+        <v>1</v>
+      </c>
+      <c r="E38">
+        <v>1024</v>
+      </c>
+      <c r="F38">
+        <v>159.794485807</v>
+      </c>
+      <c r="G38">
+        <v>82.955249071099999</v>
+      </c>
+      <c r="H38">
+        <v>362.25430393200003</v>
+      </c>
+      <c r="I38">
+        <v>107.370000124</v>
+      </c>
+      <c r="J38">
+        <v>4.6799998283399997</v>
+      </c>
+      <c r="K38" s="7">
+        <f t="shared" si="0"/>
+        <v>7.4545691015600255</v>
+      </c>
+      <c r="L38" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12">
+      <c r="A39">
+        <v>7</v>
+      </c>
+      <c r="B39" t="s">
+        <v>7</v>
+      </c>
+      <c r="C39" t="s">
+        <v>30</v>
+      </c>
+      <c r="D39">
+        <v>1</v>
+      </c>
+      <c r="E39">
+        <v>1024</v>
+      </c>
+      <c r="F39">
+        <v>164.00699496300001</v>
+      </c>
+      <c r="G39">
+        <v>94.192369937899997</v>
+      </c>
+      <c r="H39">
+        <v>315.48400592799999</v>
+      </c>
+      <c r="I39">
+        <v>46.210000038099999</v>
+      </c>
+      <c r="J39">
+        <v>2.0699999332400001</v>
+      </c>
+      <c r="K39" s="7">
+        <f t="shared" si="0"/>
+        <v>9.0046410557599188</v>
+      </c>
+      <c r="L39" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12">
+      <c r="A40">
+        <v>8</v>
+      </c>
+      <c r="B40" t="s">
+        <v>7</v>
+      </c>
+      <c r="C40" t="s">
+        <v>30</v>
+      </c>
+      <c r="D40">
+        <v>1</v>
+      </c>
+      <c r="E40">
+        <v>1024</v>
+      </c>
+      <c r="F40">
+        <v>201.021460056</v>
+      </c>
+      <c r="G40">
+        <v>91.1538639069</v>
+      </c>
+      <c r="H40">
+        <v>359.501757145</v>
+      </c>
+      <c r="I40">
+        <v>53.029999971400002</v>
+      </c>
+      <c r="J40">
+        <v>5.75</v>
+      </c>
+      <c r="K40" s="7">
+        <f t="shared" si="0"/>
+        <v>8.5464332107000018</v>
+      </c>
+      <c r="L40" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12">
+      <c r="A41">
+        <v>9</v>
+      </c>
+      <c r="B41" t="s">
+        <v>7</v>
+      </c>
+      <c r="C41" t="s">
+        <v>30</v>
+      </c>
+      <c r="D41">
+        <v>1</v>
+      </c>
+      <c r="E41">
+        <v>1024</v>
+      </c>
+      <c r="F41">
+        <v>691.71504187599999</v>
+      </c>
+      <c r="G41">
+        <v>91.696357965499999</v>
+      </c>
+      <c r="H41">
+        <v>916.97918486599997</v>
+      </c>
+      <c r="I41">
+        <v>121.769999981</v>
+      </c>
+      <c r="J41">
+        <v>4.6400001049000004</v>
+      </c>
+      <c r="K41" s="7">
+        <f t="shared" si="0"/>
+        <v>7.1577849386000025</v>
+      </c>
+      <c r="L41" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12">
+      <c r="A42">
+        <v>0</v>
+      </c>
+      <c r="B42" t="s">
+        <v>13</v>
+      </c>
+      <c r="C42" t="s">
+        <v>31</v>
+      </c>
+      <c r="D42">
+        <v>1</v>
+      </c>
+      <c r="E42">
+        <v>1024</v>
+      </c>
+      <c r="F42">
+        <v>326.00109910999998</v>
+      </c>
+      <c r="G42">
+        <v>29.4648599625</v>
+      </c>
+      <c r="H42">
+        <v>424.80244493499998</v>
+      </c>
+      <c r="I42">
+        <v>29.759999990499999</v>
+      </c>
+      <c r="J42">
+        <v>1.7799999713900001</v>
+      </c>
+      <c r="K42" s="7">
+        <f t="shared" si="0"/>
+        <v>37.796485900610037</v>
+      </c>
+      <c r="L42" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12">
+      <c r="A43">
+        <v>2</v>
+      </c>
+      <c r="B43" t="s">
+        <v>13</v>
+      </c>
+      <c r="C43" t="s">
+        <v>31</v>
+      </c>
+      <c r="D43">
+        <v>1</v>
+      </c>
+      <c r="E43">
+        <v>1024</v>
+      </c>
+      <c r="F43">
+        <v>408.57445120800003</v>
+      </c>
+      <c r="G43">
+        <v>32.547425985300002</v>
+      </c>
+      <c r="H43">
+        <v>480.344675064</v>
+      </c>
+      <c r="I43">
+        <v>22.180000066800002</v>
+      </c>
+      <c r="J43">
+        <v>3.6600000858300001</v>
+      </c>
+      <c r="K43" s="7">
+        <f t="shared" si="0"/>
+        <v>13.38279771806998</v>
+      </c>
+      <c r="L43" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12">
+      <c r="A44">
+        <v>5</v>
+      </c>
+      <c r="B44" t="s">
+        <v>13</v>
+      </c>
+      <c r="C44" t="s">
+        <v>32</v>
+      </c>
+      <c r="D44">
+        <v>1</v>
+      </c>
+      <c r="E44">
+        <v>1024</v>
+      </c>
+      <c r="F44">
+        <v>1708.15698195</v>
+      </c>
+      <c r="G44">
+        <v>35.188234090800002</v>
+      </c>
+      <c r="H44">
+        <v>2211.25476789</v>
+      </c>
+      <c r="I44">
+        <v>455.17000007600001</v>
+      </c>
+      <c r="J44">
+        <v>1.0699999332400001</v>
+      </c>
+      <c r="K44" s="7">
+        <f t="shared" si="0"/>
+        <v>11.669551839959695</v>
+      </c>
+      <c r="L44" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12">
+      <c r="A45">
+        <v>6</v>
+      </c>
+      <c r="B45" t="s">
+        <v>13</v>
+      </c>
+      <c r="C45" t="s">
+        <v>32</v>
+      </c>
+      <c r="D45">
+        <v>1</v>
+      </c>
+      <c r="E45">
+        <v>1024</v>
+      </c>
+      <c r="F45">
+        <v>723.18473601300002</v>
+      </c>
+      <c r="G45">
+        <v>33.547902107200002</v>
+      </c>
+      <c r="H45">
+        <v>819.20431399300003</v>
+      </c>
+      <c r="I45">
+        <v>49.309999942799998</v>
+      </c>
+      <c r="J45">
+        <v>2.0299999713900001</v>
+      </c>
+      <c r="K45" s="7">
+        <f t="shared" si="0"/>
+        <v>11.131675958610003</v>
+      </c>
+      <c r="L45" t="s">
+        <v>33</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L32">
+  <autoFilter ref="A1:L31">
     <filterColumn colId="1">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>

</xml_diff>

<commit_message>
included Melissa's data in figure 6
git-svn-id: file://localhost/tmp/svn2git/svn@7704 defb5e50-622e-49ec-a68e-d72c7db87b45
</commit_message>
<xml_diff>
--- a/papers/ccpe-cloud12/performance/pd.xlsx
+++ b/papers/ccpe-cloud12/performance/pd.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22416"/>
   <workbookPr showInkAnnotation="0" hidePivotFieldList="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="48460" windowHeight="28360" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="26600" windowHeight="14920" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Blatt1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
   </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <pivotCaches>
-    <pivotCache cacheId="9" r:id="rId2"/>
+    <pivotCache cacheId="28" r:id="rId2"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="38">
   <si>
     <t>Run</t>
   </si>
@@ -150,12 +150,6 @@
     <t>Delta Runtime</t>
   </si>
   <si>
-    <t>Upload</t>
-  </si>
-  <si>
-    <t>Download</t>
-  </si>
-  <si>
     <t>s3://pilot-data-e80f3c86-f53f-11e1-999d-00215ec9e3ac</t>
   </si>
   <si>
@@ -172,6 +166,18 @@
   </si>
   <si>
     <t xml:space="preserve">CU Compute </t>
+  </si>
+  <si>
+    <t>Download (Cloud Storage - VM)</t>
+  </si>
+  <si>
+    <t>Upload (FG - Cloud Storage)</t>
+  </si>
+  <si>
+    <t>walrus</t>
+  </si>
+  <si>
+    <t>euca://india.futuregrid.org</t>
   </si>
 </sst>
 </file>
@@ -267,13 +273,7 @@
     <cellStyle name="Link" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <numFmt numFmtId="164" formatCode="0.0"/>
     </dxf>
@@ -312,7 +312,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Upload</c:v>
+                  <c:v>Upload (FG - Cloud Storage)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -328,29 +328,35 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Blatt1!$O$18:$O$19</c:f>
+              <c:f>Blatt1!$O$18:$O$20</c:f>
               <c:strCache>
-                <c:ptCount val="2"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>ec2+ssh://aws.amazon.com/</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>gce+ssh://google.com</c:v>
                 </c:pt>
+                <c:pt idx="2">
+                  <c:v>euca://india.futuregrid.org</c:v>
+                </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Blatt1!$P$18:$P$19</c:f>
+              <c:f>Blatt1!$P$18:$P$20</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
-                <c:ptCount val="2"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>220.7107000827</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>791.47931707025</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>21.72547779082</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -365,7 +371,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Download</c:v>
+                  <c:v>Download (Cloud Storage - VM)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -381,29 +387,35 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Blatt1!$O$18:$O$19</c:f>
+              <c:f>Blatt1!$O$18:$O$20</c:f>
               <c:strCache>
-                <c:ptCount val="2"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>ec2+ssh://aws.amazon.com/</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>gce+ssh://google.com</c:v>
                 </c:pt>
+                <c:pt idx="2">
+                  <c:v>euca://india.futuregrid.org</c:v>
+                </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Blatt1!$Q$18:$Q$19</c:f>
+              <c:f>Blatt1!$Q$18:$Q$20</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
-                <c:ptCount val="2"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>110.47700002196</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>139.105000019025</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15.09400000574</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -477,29 +489,35 @@
           </c:errBars>
           <c:cat>
             <c:strRef>
-              <c:f>Blatt1!$O$18:$O$19</c:f>
+              <c:f>Blatt1!$O$18:$O$20</c:f>
               <c:strCache>
-                <c:ptCount val="2"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>ec2+ssh://aws.amazon.com/</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>gce+ssh://google.com</c:v>
                 </c:pt>
+                <c:pt idx="2">
+                  <c:v>euca://india.futuregrid.org</c:v>
+                </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Blatt1!$R$18:$R$19</c:f>
+              <c:f>Blatt1!$R$18:$R$20</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
-                <c:ptCount val="2"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>74.09683890343001</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>32.68710553645</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>302.40736880304</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -529,29 +547,35 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Blatt1!$O$18:$O$19</c:f>
+              <c:f>Blatt1!$O$18:$O$20</c:f>
               <c:strCache>
-                <c:ptCount val="2"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>ec2+ssh://aws.amazon.com/</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>gce+ssh://google.com</c:v>
                 </c:pt>
+                <c:pt idx="2">
+                  <c:v>euca://india.futuregrid.org</c:v>
+                </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Blatt1!$T$18:$T$19</c:f>
+              <c:f>Blatt1!$T$18:$T$20</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
-                <c:ptCount val="2"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>3.2009999990462</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>2.1349999904625</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.776000022888</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -711,18 +735,20 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Andre Luckow" refreshedDate="41156.362004629627" createdVersion="4" refreshedVersion="4" minRefreshableVersion="3" recordCount="44">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Andre Luckow" refreshedDate="41158.786918287034" createdVersion="4" refreshedVersion="4" minRefreshableVersion="3" recordCount="49">
   <cacheSource type="worksheet">
-    <worksheetSource ref="A1:L45" sheet="Blatt1"/>
+    <worksheetSource ref="A1:L50" sheet="Blatt1"/>
   </cacheSource>
   <cacheFields count="12">
     <cacheField name="Run" numFmtId="0">
       <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="0" maxValue="9"/>
     </cacheField>
     <cacheField name="PC" numFmtId="0">
-      <sharedItems count="2">
+      <sharedItems count="4">
         <s v="ec2+ssh://aws.amazon.com/"/>
         <s v="gce+ssh://google.com"/>
+        <s v="euca://india.futuregrid.org"/>
+        <s v="euca" u="1"/>
       </sharedItems>
     </cacheField>
     <cacheField name="PD" numFmtId="0">
@@ -732,16 +758,17 @@
       <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="1"/>
     </cacheField>
     <cacheField name="MB" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="128" maxValue="1024" count="2">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="128" maxValue="8192" count="3">
         <n v="1024"/>
         <n v="128"/>
+        <n v="8192" u="1"/>
       </sharedItems>
     </cacheField>
     <cacheField name="Upload Time" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="17.992821216599999" maxValue="2002.243119"/>
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="16.788008928300002" maxValue="2002.243119"/>
     </cacheField>
     <cacheField name="Pilot Queue" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="29.4648599625" maxValue="94.932879924800005"/>
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="29.4648599625" maxValue="575.899488926"/>
     </cacheField>
     <cacheField name="Total Runtime" numFmtId="0">
       <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="99.422956943499997" maxValue="2211.25476789"/>
@@ -771,7 +798,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="44">
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="49">
   <r>
     <n v="0"/>
     <x v="0"/>
@@ -1388,27 +1415,100 @@
     <n v="11.131675958610003"/>
     <x v="1"/>
   </r>
+  <r>
+    <n v="1"/>
+    <x v="2"/>
+    <s v="walrus"/>
+    <n v="1"/>
+    <x v="0"/>
+    <n v="29.707263946499999"/>
+    <n v="64.187892198599997"/>
+    <n v="124.951183081"/>
+    <n v="18.379999875999999"/>
+    <n v="3.92000007629"/>
+    <n v="8.7560269836099991"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="2"/>
+    <x v="2"/>
+    <s v="walrus"/>
+    <n v="1"/>
+    <x v="0"/>
+    <n v="23.4599649906"/>
+    <n v="53.7772819996"/>
+    <n v="102.28686881100001"/>
+    <n v="14.9800000191"/>
+    <n v="1.44000005722"/>
+    <n v="8.629621744480005"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="3"/>
+    <x v="2"/>
+    <s v="walrus"/>
+    <n v="1"/>
+    <x v="0"/>
+    <n v="16.788008928300002"/>
+    <n v="377.41170692399999"/>
+    <n v="417.24973487900002"/>
+    <n v="13.9300000668"/>
+    <n v="1.6699998378799998"/>
+    <n v="7.4500191220200236"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="4"/>
+    <x v="2"/>
+    <s v="walrus"/>
+    <n v="1"/>
+    <x v="0"/>
+    <n v="21.6351509094"/>
+    <n v="440.760473967"/>
+    <n v="489.46177983299998"/>
+    <n v="14.170000076299999"/>
+    <n v="4.3199999332400001"/>
+    <n v="8.5761549470599903"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="5"/>
+    <x v="2"/>
+    <s v="walrus"/>
+    <n v="1"/>
+    <x v="0"/>
+    <n v="17.037000179300001"/>
+    <n v="575.899488926"/>
+    <n v="617.99924611999995"/>
+    <n v="14.009999990500001"/>
+    <n v="2.5300002098099998"/>
+    <n v="8.5227568143899362"/>
+    <x v="1"/>
+  </r>
 </pivotCacheRecords>
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="9" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0" rowHeaderCaption="">
-  <location ref="O16:U20" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="2" colPageCount="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="28" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0" rowHeaderCaption="">
+  <location ref="O16:U21" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="2" colPageCount="1"/>
   <pivotFields count="12">
     <pivotField showAll="0"/>
     <pivotField axis="axisRow" showAll="0">
-      <items count="3">
+      <items count="5">
         <item x="0"/>
         <item x="1"/>
+        <item m="1" x="3"/>
+        <item x="2"/>
         <item t="default"/>
       </items>
     </pivotField>
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
-      <items count="3">
+      <items count="4">
         <item h="1" x="1"/>
         <item x="0"/>
+        <item h="1" m="1" x="2"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -1428,12 +1528,15 @@
   <rowFields count="1">
     <field x="1"/>
   </rowFields>
-  <rowItems count="3">
+  <rowItems count="4">
     <i>
       <x/>
     </i>
     <i>
       <x v="1"/>
+    </i>
+    <i>
+      <x v="3"/>
     </i>
     <i t="grand">
       <x/>
@@ -1467,15 +1570,15 @@
     <pageField fld="11" hier="-1"/>
   </pageFields>
   <dataFields count="6">
-    <dataField name="Upload" fld="5" subtotal="average" baseField="0" baseItem="0"/>
-    <dataField name="Download" fld="8" subtotal="average" baseField="0" baseItem="0"/>
+    <dataField name="Upload (FG - Cloud Storage)" fld="5" subtotal="average" baseField="0" baseItem="0"/>
+    <dataField name="Download (Cloud Storage - VM)" fld="8" subtotal="average" baseField="0" baseItem="0"/>
     <dataField name="Pilot Queue " fld="6" subtotal="average" baseField="0" baseItem="0"/>
     <dataField name="Mittelwert - Total Runtime" fld="7" subtotal="average" baseField="0" baseItem="0"/>
     <dataField name="CU Compute " fld="9" subtotal="average" baseField="0" baseItem="0"/>
     <dataField name="STABW - Total Runtime" fld="7" subtotal="stdDev" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="1">
-    <format dxfId="2">
+    <format dxfId="0">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
   </formats>
@@ -1819,10 +1922,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1:W45"/>
+  <dimension ref="A1:W50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AB25" sqref="AB25"/>
+    <sheetView tabSelected="1" topLeftCell="L33" workbookViewId="0">
+      <selection activeCell="X62" sqref="X62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1830,14 +1933,14 @@
     <col min="1" max="1" width="2.1640625" customWidth="1"/>
     <col min="2" max="2" width="24.6640625" customWidth="1"/>
     <col min="3" max="3" width="47.6640625" customWidth="1"/>
-    <col min="4" max="4" width="2.1640625" customWidth="1"/>
+    <col min="4" max="4" width="4" customWidth="1"/>
     <col min="5" max="5" width="5.1640625" bestFit="1" customWidth="1"/>
     <col min="6" max="8" width="12.1640625" customWidth="1"/>
     <col min="9" max="10" width="12.1640625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12.1640625" style="8" customWidth="1"/>
     <col min="15" max="15" width="24.6640625" customWidth="1"/>
-    <col min="16" max="16" width="15.83203125" customWidth="1"/>
-    <col min="17" max="17" width="9.5" customWidth="1"/>
+    <col min="16" max="16" width="23.83203125" customWidth="1"/>
+    <col min="17" max="17" width="27" customWidth="1"/>
     <col min="18" max="18" width="11.1640625" customWidth="1"/>
     <col min="19" max="19" width="23" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="12" customWidth="1"/>
@@ -2398,7 +2501,7 @@
         <v>22</v>
       </c>
       <c r="P14" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="15" spans="1:16">
@@ -2524,19 +2627,19 @@
         <v>26</v>
       </c>
       <c r="P17" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="Q17" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="R17" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="S17" t="s">
         <v>24</v>
       </c>
       <c r="T17" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="U17" t="s">
         <v>25</v>
@@ -2705,25 +2808,25 @@
         <v>23</v>
       </c>
       <c r="O20" s="4" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="P20" s="5">
-        <v>383.7874477934285</v>
+        <v>21.725477790820001</v>
       </c>
       <c r="Q20" s="5">
-        <v>118.65642859255</v>
+        <v>15.09400000574</v>
       </c>
       <c r="R20" s="5">
-        <v>62.2654865128643</v>
+        <v>302.40736880303996</v>
       </c>
       <c r="S20" s="5">
-        <v>579.05295133557138</v>
+        <v>350.38976254479996</v>
       </c>
       <c r="T20" s="5">
-        <v>2.896428568022285</v>
+        <v>2.7760000228879997</v>
       </c>
       <c r="U20" s="5">
-        <v>512.94119542916803</v>
+        <v>227.92746465831291</v>
       </c>
     </row>
     <row r="21" spans="1:23">
@@ -2764,6 +2867,27 @@
       <c r="L21" t="s">
         <v>23</v>
       </c>
+      <c r="O21" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="P21" s="5">
+        <v>288.50798200326835</v>
+      </c>
+      <c r="Q21" s="5">
+        <v>91.403157911810538</v>
+      </c>
+      <c r="R21" s="5">
+        <v>125.46071869448947</v>
+      </c>
+      <c r="S21" s="5">
+        <v>518.87842796957887</v>
+      </c>
+      <c r="T21" s="5">
+        <v>2.8647368456185256</v>
+      </c>
+      <c r="U21" s="5">
+        <v>460.72721525177963</v>
+      </c>
     </row>
     <row r="22" spans="1:23">
       <c r="A22">
@@ -3163,7 +3287,7 @@
         <v>7</v>
       </c>
       <c r="C32" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D32">
         <v>1</v>
@@ -3191,7 +3315,7 @@
         <v>8.8520209790299873</v>
       </c>
       <c r="L32" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="33" spans="1:12">
@@ -3202,7 +3326,7 @@
         <v>7</v>
       </c>
       <c r="C33" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D33">
         <v>1</v>
@@ -3230,7 +3354,7 @@
         <v>8.3799438480299955</v>
       </c>
       <c r="L33" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="34" spans="1:12">
@@ -3241,7 +3365,7 @@
         <v>7</v>
       </c>
       <c r="C34" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D34">
         <v>1</v>
@@ -3269,7 +3393,7 @@
         <v>13.464279890249998</v>
       </c>
       <c r="L34" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="35" spans="1:12">
@@ -3280,7 +3404,7 @@
         <v>7</v>
       </c>
       <c r="C35" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D35">
         <v>1</v>
@@ -3308,7 +3432,7 @@
         <v>8.4689979554199795</v>
       </c>
       <c r="L35" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="36" spans="1:12">
@@ -3319,7 +3443,7 @@
         <v>7</v>
       </c>
       <c r="C36" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D36">
         <v>1</v>
@@ -3347,7 +3471,7 @@
         <v>7.7552559369980258</v>
       </c>
       <c r="L36" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="37" spans="1:12">
@@ -3358,7 +3482,7 @@
         <v>7</v>
       </c>
       <c r="C37" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D37">
         <v>1</v>
@@ -3386,7 +3510,7 @@
         <v>7.195799828289978</v>
       </c>
       <c r="L37" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="38" spans="1:12">
@@ -3397,7 +3521,7 @@
         <v>7</v>
       </c>
       <c r="C38" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D38">
         <v>1</v>
@@ -3425,7 +3549,7 @@
         <v>7.4545691015600255</v>
       </c>
       <c r="L38" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="39" spans="1:12">
@@ -3436,7 +3560,7 @@
         <v>7</v>
       </c>
       <c r="C39" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D39">
         <v>1</v>
@@ -3464,7 +3588,7 @@
         <v>9.0046410557599188</v>
       </c>
       <c r="L39" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="40" spans="1:12">
@@ -3475,7 +3599,7 @@
         <v>7</v>
       </c>
       <c r="C40" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D40">
         <v>1</v>
@@ -3503,7 +3627,7 @@
         <v>8.5464332107000018</v>
       </c>
       <c r="L40" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="41" spans="1:12">
@@ -3514,7 +3638,7 @@
         <v>7</v>
       </c>
       <c r="C41" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D41">
         <v>1</v>
@@ -3542,7 +3666,7 @@
         <v>7.1577849386000025</v>
       </c>
       <c r="L41" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="42" spans="1:12">
@@ -3553,7 +3677,7 @@
         <v>13</v>
       </c>
       <c r="C42" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D42">
         <v>1</v>
@@ -3581,7 +3705,7 @@
         <v>37.796485900610037</v>
       </c>
       <c r="L42" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="43" spans="1:12">
@@ -3592,7 +3716,7 @@
         <v>13</v>
       </c>
       <c r="C43" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D43">
         <v>1</v>
@@ -3620,7 +3744,7 @@
         <v>13.38279771806998</v>
       </c>
       <c r="L43" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="44" spans="1:12">
@@ -3631,7 +3755,7 @@
         <v>13</v>
       </c>
       <c r="C44" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D44">
         <v>1</v>
@@ -3659,7 +3783,7 @@
         <v>11.669551839959695</v>
       </c>
       <c r="L44" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="45" spans="1:12">
@@ -3670,7 +3794,7 @@
         <v>13</v>
       </c>
       <c r="C45" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D45">
         <v>1</v>
@@ -3698,7 +3822,202 @@
         <v>11.131675958610003</v>
       </c>
       <c r="L45" t="s">
-        <v>33</v>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12">
+      <c r="A46">
+        <v>1</v>
+      </c>
+      <c r="B46" t="s">
+        <v>37</v>
+      </c>
+      <c r="C46" t="s">
+        <v>36</v>
+      </c>
+      <c r="D46">
+        <v>1</v>
+      </c>
+      <c r="E46">
+        <v>1024</v>
+      </c>
+      <c r="F46">
+        <v>29.707263946499999</v>
+      </c>
+      <c r="G46">
+        <v>64.187892198599997</v>
+      </c>
+      <c r="H46">
+        <v>124.951183081</v>
+      </c>
+      <c r="I46">
+        <v>18.379999875999999</v>
+      </c>
+      <c r="J46">
+        <v>3.92000007629</v>
+      </c>
+      <c r="K46" s="7">
+        <f t="shared" ref="K46:K50" si="1">H46-(SUM(F46,G46,I46,J46))</f>
+        <v>8.7560269836099991</v>
+      </c>
+      <c r="L46" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12">
+      <c r="A47">
+        <v>2</v>
+      </c>
+      <c r="B47" t="s">
+        <v>37</v>
+      </c>
+      <c r="C47" t="s">
+        <v>36</v>
+      </c>
+      <c r="D47">
+        <v>1</v>
+      </c>
+      <c r="E47">
+        <v>1024</v>
+      </c>
+      <c r="F47">
+        <v>23.4599649906</v>
+      </c>
+      <c r="G47">
+        <v>53.7772819996</v>
+      </c>
+      <c r="H47">
+        <v>102.28686881100001</v>
+      </c>
+      <c r="I47">
+        <v>14.9800000191</v>
+      </c>
+      <c r="J47">
+        <v>1.44000005722</v>
+      </c>
+      <c r="K47" s="7">
+        <f t="shared" si="1"/>
+        <v>8.629621744480005</v>
+      </c>
+      <c r="L47" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12">
+      <c r="A48">
+        <v>3</v>
+      </c>
+      <c r="B48" t="s">
+        <v>37</v>
+      </c>
+      <c r="C48" t="s">
+        <v>36</v>
+      </c>
+      <c r="D48">
+        <v>1</v>
+      </c>
+      <c r="E48">
+        <v>1024</v>
+      </c>
+      <c r="F48">
+        <v>16.788008928300002</v>
+      </c>
+      <c r="G48">
+        <v>377.41170692399999</v>
+      </c>
+      <c r="H48">
+        <v>417.24973487900002</v>
+      </c>
+      <c r="I48">
+        <v>13.9300000668</v>
+      </c>
+      <c r="J48">
+        <v>1.6699998378799998</v>
+      </c>
+      <c r="K48" s="7">
+        <f t="shared" si="1"/>
+        <v>7.4500191220200236</v>
+      </c>
+      <c r="L48" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12">
+      <c r="A49">
+        <v>4</v>
+      </c>
+      <c r="B49" t="s">
+        <v>37</v>
+      </c>
+      <c r="C49" t="s">
+        <v>36</v>
+      </c>
+      <c r="D49">
+        <v>1</v>
+      </c>
+      <c r="E49">
+        <v>1024</v>
+      </c>
+      <c r="F49">
+        <v>21.6351509094</v>
+      </c>
+      <c r="G49">
+        <v>440.760473967</v>
+      </c>
+      <c r="H49">
+        <v>489.46177983299998</v>
+      </c>
+      <c r="I49">
+        <v>14.170000076299999</v>
+      </c>
+      <c r="J49">
+        <v>4.3199999332400001</v>
+      </c>
+      <c r="K49" s="7">
+        <f t="shared" si="1"/>
+        <v>8.5761549470599903</v>
+      </c>
+      <c r="L49" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12">
+      <c r="A50">
+        <v>5</v>
+      </c>
+      <c r="B50" t="s">
+        <v>37</v>
+      </c>
+      <c r="C50" t="s">
+        <v>36</v>
+      </c>
+      <c r="D50">
+        <v>1</v>
+      </c>
+      <c r="E50">
+        <v>1024</v>
+      </c>
+      <c r="F50">
+        <v>17.037000179300001</v>
+      </c>
+      <c r="G50">
+        <v>575.899488926</v>
+      </c>
+      <c r="H50">
+        <v>617.99924611999995</v>
+      </c>
+      <c r="I50">
+        <v>14.009999990500001</v>
+      </c>
+      <c r="J50">
+        <v>2.5300002098099998</v>
+      </c>
+      <c r="K50" s="7">
+        <f t="shared" si="1"/>
+        <v>8.5227568143899362</v>
+      </c>
+      <c r="L50" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
some work on section 3 left some comments for Pradeep to address in section 5
git-svn-id: file://localhost/tmp/svn2git/svn@7708 defb5e50-622e-49ec-a68e-d72c7db87b45
</commit_message>
<xml_diff>
--- a/papers/ccpe-cloud12/performance/pd.xlsx
+++ b/papers/ccpe-cloud12/performance/pd.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22416"/>
   <workbookPr showInkAnnotation="0" hidePivotFieldList="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="26600" windowHeight="14920" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="50480" windowHeight="28360" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Blatt1" sheetId="1" r:id="rId1"/>
@@ -273,7 +273,16 @@
     <cellStyle name="Link" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="4">
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="0.0"/>
     </dxf>
@@ -335,10 +344,10 @@
                   <c:v>ec2+ssh://aws.amazon.com/</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>gce+ssh://google.com</c:v>
+                  <c:v>euca://india.futuregrid.org</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>euca://india.futuregrid.org</c:v>
+                  <c:v>gce+ssh://google.com</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -353,10 +362,10 @@
                   <c:v>220.7107000827</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>791.47931707025</c:v>
+                  <c:v>21.72547779082</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>21.72547779082</c:v>
+                  <c:v>791.47931707025</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -394,10 +403,10 @@
                   <c:v>ec2+ssh://aws.amazon.com/</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>gce+ssh://google.com</c:v>
+                  <c:v>euca://india.futuregrid.org</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>euca://india.futuregrid.org</c:v>
+                  <c:v>gce+ssh://google.com</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -412,10 +421,10 @@
                   <c:v>110.47700002196</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>139.105000019025</c:v>
+                  <c:v>15.09400000574</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>15.09400000574</c:v>
+                  <c:v>139.105000019025</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -449,14 +458,17 @@
             <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
-                <c:f>Blatt1!$U$18:$U$19</c:f>
+                <c:f>Blatt1!$U$18:$U$20</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="2"/>
+                  <c:ptCount val="3"/>
                   <c:pt idx="0">
                     <c:v>211.5752818356191</c:v>
                   </c:pt>
                   <c:pt idx="1">
+                    <c:v>227.927464658313</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
                     <c:v>836.5967639974622</c:v>
                   </c:pt>
                 </c:numCache>
@@ -464,14 +476,17 @@
             </c:plus>
             <c:minus>
               <c:numRef>
-                <c:f>Blatt1!$U$18:$U$19</c:f>
+                <c:f>Blatt1!$U$18:$U$20</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="2"/>
+                  <c:ptCount val="3"/>
                   <c:pt idx="0">
                     <c:v>211.5752818356191</c:v>
                   </c:pt>
                   <c:pt idx="1">
+                    <c:v>227.927464658313</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
                     <c:v>836.5967639974622</c:v>
                   </c:pt>
                 </c:numCache>
@@ -496,10 +511,10 @@
                   <c:v>ec2+ssh://aws.amazon.com/</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>gce+ssh://google.com</c:v>
+                  <c:v>euca://india.futuregrid.org</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>euca://india.futuregrid.org</c:v>
+                  <c:v>gce+ssh://google.com</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -514,10 +529,10 @@
                   <c:v>74.09683890343001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>32.68710553645</c:v>
+                  <c:v>302.40736880304</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>302.40736880304</c:v>
+                  <c:v>32.68710553645</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -554,10 +569,10 @@
                   <c:v>ec2+ssh://aws.amazon.com/</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>gce+ssh://google.com</c:v>
+                  <c:v>euca://india.futuregrid.org</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>euca://india.futuregrid.org</c:v>
+                  <c:v>gce+ssh://google.com</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -572,10 +587,10 @@
                   <c:v>3.2009999990462</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.1349999904625</c:v>
+                  <c:v>2.776000022888</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.776000022888</c:v>
+                  <c:v>2.1349999904625</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1493,12 +1508,12 @@
   <location ref="O16:U21" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="2" colPageCount="1"/>
   <pivotFields count="12">
     <pivotField showAll="0"/>
-    <pivotField axis="axisRow" showAll="0">
+    <pivotField axis="axisRow" showAll="0" sortType="ascending">
       <items count="5">
         <item x="0"/>
-        <item x="1"/>
         <item m="1" x="3"/>
         <item x="2"/>
+        <item x="1"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -1533,7 +1548,7 @@
       <x/>
     </i>
     <i>
-      <x v="1"/>
+      <x v="2"/>
     </i>
     <i>
       <x v="3"/>
@@ -1578,7 +1593,7 @@
     <dataField name="STABW - Total Runtime" fld="7" subtotal="stdDev" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="1">
-    <format dxfId="0">
+    <format dxfId="3">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
   </formats>
@@ -1924,8 +1939,8 @@
   <sheetPr filterMode="1" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:W50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L33" workbookViewId="0">
-      <selection activeCell="X62" sqref="X62"/>
+    <sheetView tabSelected="1" topLeftCell="L4" workbookViewId="0">
+      <selection activeCell="AL26" sqref="AL26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2744,29 +2759,29 @@
         <v>23</v>
       </c>
       <c r="O19" s="4" t="s">
-        <v>13</v>
+        <v>37</v>
       </c>
       <c r="P19" s="5">
-        <v>791.47931707024998</v>
+        <v>21.725477790820001</v>
       </c>
       <c r="Q19" s="5">
-        <v>139.105000019025</v>
+        <v>15.09400000574</v>
       </c>
       <c r="R19" s="5">
-        <v>32.687105536450005</v>
+        <v>302.40736880303996</v>
       </c>
       <c r="S19" s="5">
-        <v>983.90155047050007</v>
+        <v>350.38976254479996</v>
       </c>
       <c r="T19" s="5">
-        <v>2.1349999904625001</v>
+        <v>2.7760000228879997</v>
       </c>
       <c r="U19" s="5">
-        <v>836.59676399746229</v>
+        <v>227.92746465831291</v>
       </c>
       <c r="W19">
         <f>P19/P18</f>
-        <v>3.5860486907688833</v>
+        <v>9.8434184580446241E-2</v>
       </c>
     </row>
     <row r="20" spans="1:23">
@@ -2808,25 +2823,25 @@
         <v>23</v>
       </c>
       <c r="O20" s="4" t="s">
-        <v>37</v>
+        <v>13</v>
       </c>
       <c r="P20" s="5">
-        <v>21.725477790820001</v>
+        <v>791.47931707024998</v>
       </c>
       <c r="Q20" s="5">
-        <v>15.09400000574</v>
+        <v>139.105000019025</v>
       </c>
       <c r="R20" s="5">
-        <v>302.40736880303996</v>
+        <v>32.687105536450005</v>
       </c>
       <c r="S20" s="5">
-        <v>350.38976254479996</v>
+        <v>983.90155047050007</v>
       </c>
       <c r="T20" s="5">
-        <v>2.7760000228879997</v>
+        <v>2.1349999904625001</v>
       </c>
       <c r="U20" s="5">
-        <v>227.92746465831291</v>
+        <v>836.59676399746229</v>
       </c>
     </row>
     <row r="21" spans="1:23">
@@ -2871,13 +2886,13 @@
         <v>17</v>
       </c>
       <c r="P21" s="5">
-        <v>288.50798200326835</v>
+        <v>288.50798200326841</v>
       </c>
       <c r="Q21" s="5">
         <v>91.403157911810538</v>
       </c>
       <c r="R21" s="5">
-        <v>125.46071869448947</v>
+        <v>125.46071869448949</v>
       </c>
       <c r="S21" s="5">
         <v>518.87842796957887</v>
@@ -2886,7 +2901,7 @@
         <v>2.8647368456185256</v>
       </c>
       <c r="U21" s="5">
-        <v>460.72721525177963</v>
+        <v>460.72721525177974</v>
       </c>
     </row>
     <row r="22" spans="1:23">

</xml_diff>

<commit_message>
udpate to figure 6
git-svn-id: file://localhost/tmp/svn2git/svn@7718 defb5e50-622e-49ec-a68e-d72c7db87b45
</commit_message>
<xml_diff>
--- a/papers/ccpe-cloud12/performance/pd.xlsx
+++ b/papers/ccpe-cloud12/performance/pd.xlsx
@@ -18,7 +18,7 @@
   </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <pivotCaches>
-    <pivotCache cacheId="9" r:id="rId3"/>
+    <pivotCache cacheId="0" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -364,6 +364,11 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF000000"/>
+    </mruColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -405,8 +410,8 @@
           <c:spPr>
             <a:solidFill>
               <a:schemeClr val="tx1">
-                <a:lumMod val="85000"/>
-                <a:lumOff val="15000"/>
+                <a:lumMod val="75000"/>
+                <a:lumOff val="25000"/>
               </a:schemeClr>
             </a:solidFill>
           </c:spPr>
@@ -630,9 +635,7 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="bg1">
-                <a:lumMod val="85000"/>
-              </a:schemeClr>
+              <a:srgbClr val="000000"/>
             </a:solidFill>
           </c:spPr>
           <c:invertIfNegative val="0"/>
@@ -682,11 +685,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="2078165000"/>
-        <c:axId val="2078168136"/>
+        <c:axId val="2128509784"/>
+        <c:axId val="2128512808"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2078165000"/>
+        <c:axId val="2128509784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -705,7 +708,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2078168136"/>
+        <c:crossAx val="2128512808"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -713,7 +716,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2078168136"/>
+        <c:axId val="2128512808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -753,7 +756,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2078165000"/>
+        <c:crossAx val="2128509784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1678,7 +1681,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="9" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0" rowHeaderCaption="">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0" rowHeaderCaption="">
   <location ref="O16:U22" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="2" colPageCount="1"/>
   <pivotFields count="12">
     <pivotField showAll="0"/>
@@ -1784,11 +1787,11 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pd" connectionId="3" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pd_random" connectionId="2" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pd_random" connectionId="2" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pd" connectionId="3" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2121,7 +2124,7 @@
   <dimension ref="A1:W57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O17" sqref="O17"/>
+      <selection activeCell="T72" sqref="T72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4278,7 +4281,7 @@
         <v>3.36800001264</v>
       </c>
       <c r="K51" s="7">
-        <f>H51-(SUM(F51,G51,I51,J51))</f>
+        <f t="shared" ref="K51:K57" si="2">H51-(SUM(F51,G51,I51,J51))</f>
         <v>1003.2050159537603</v>
       </c>
       <c r="L51" t="s">
@@ -4317,7 +4320,7 @@
         <v>2.8239999949899999</v>
       </c>
       <c r="K52" s="7">
-        <f>H52-(SUM(F52,G52,I52,J52))</f>
+        <f t="shared" si="2"/>
         <v>931.98281388240957</v>
       </c>
       <c r="L52" t="s">
@@ -4356,7 +4359,7 @@
         <v>3.15425001383</v>
       </c>
       <c r="K53" s="7">
-        <f>H53-(SUM(F53,G53,I53,J53))</f>
+        <f t="shared" si="2"/>
         <v>1041.1296799831698</v>
       </c>
       <c r="L53" t="s">
@@ -4395,7 +4398,7 @@
         <v>3.1137499928499999</v>
       </c>
       <c r="K54" s="7">
-        <f>H54-(SUM(F54,G54,I54,J54))</f>
+        <f t="shared" si="2"/>
         <v>1011.4563330004503</v>
       </c>
       <c r="L54" t="s">
@@ -4434,7 +4437,7 @@
         <v>2.8917499959500002</v>
       </c>
       <c r="K55" s="7">
-        <f>H55-(SUM(F55,G55,I55,J55))</f>
+        <f t="shared" si="2"/>
         <v>1395.8635980072499</v>
       </c>
       <c r="L55" t="s">
@@ -4473,7 +4476,7 @@
         <v>2.2719999671000002</v>
       </c>
       <c r="K56" s="7">
-        <f>H56-(SUM(F56,G56,I56,J56))</f>
+        <f t="shared" si="2"/>
         <v>1087.4554550176003</v>
       </c>
       <c r="L56" t="s">
@@ -4512,7 +4515,7 @@
         <v>6.9882500290899996</v>
       </c>
       <c r="K57" s="7">
-        <f>H57-(SUM(F57,G57,I57,J57))</f>
+        <f t="shared" si="2"/>
         <v>1000.7751201542096</v>
       </c>
       <c r="L57" t="s">

</xml_diff>

<commit_message>
new performance data. Attempt to improve intro to performance section
git-svn-id: file://localhost/tmp/svn2git/svn@7726 defb5e50-622e-49ec-a68e-d72c7db87b45
</commit_message>
<xml_diff>
--- a/papers/ccpe-cloud12/performance/pd.xlsx
+++ b/papers/ccpe-cloud12/performance/pd.xlsx
@@ -14,11 +14,13 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'1 CU'!$A$1:$L$31</definedName>
     <definedName name="pd" localSheetId="0">'1 CU'!$A$1:$J$31</definedName>
     <definedName name="pd_multi_cu" localSheetId="1">'n CUs'!$A$1:$J$1</definedName>
+    <definedName name="pd_multi_cu_1" localSheetId="0">'1 CU'!$A$51:$J$68</definedName>
+    <definedName name="pd_multi_cu_1" localSheetId="1">'n CUs'!$A$2:$J$22</definedName>
     <definedName name="pd_random" localSheetId="0">'1 CU'!$A$32:$J$45</definedName>
   </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId3"/>
+    <pivotCache cacheId="4" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -46,7 +48,23 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="2" name="pd_random.csv" type="6" refreshedVersion="0" background="1" saveData="1">
+  <connection id="2" name="pd_multi_cu.txt1" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" sourceFile="Macintosh HD:Users:luckow:Dropbox:SAGA:papers:ccpe-cloud12:performance:pd_multi_cu.txt" comma="1">
+      <textFields count="10">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="3" name="pd_random.csv" type="6" refreshedVersion="0" background="1" saveData="1">
     <textPr fileType="mac" sourceFile="Macintosh HD:Users:luckow:Dropbox:SAGA:papers:ccpe-cloud12:performance:pd_random.csv" comma="1">
       <textFields count="10">
         <textField/>
@@ -62,7 +80,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="3" name="pd.csv" type="6" refreshedVersion="0" background="1" saveData="1">
+  <connection id="4" name="pd.csv" type="6" refreshedVersion="0" background="1" saveData="1">
     <textPr fileType="mac" sourceFile="Macintosh HD:Users:luckow:Dropbox:SAGA:papers:ccpe-cloud12:performance:pd.csv" comma="1" qualifier="none">
       <textFields count="10">
         <textField/>
@@ -82,7 +100,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="52">
   <si>
     <t>Run</t>
   </si>
@@ -225,7 +243,21 @@
     <t>Google</t>
   </si>
   <si>
-    <t>gce+ssh://google.com (multi cu)</t>
+    <t>s3://pilot-data-a84f6250-f99b-11e1-818a-02215ecdd90b</t>
+  </si>
+  <si>
+    <t>Google (Multi CU)</t>
+  </si>
+  <si>
+    <t>Amazon (Multi CU)</t>
+  </si>
+  <si>
+    <t>Amazon
+(40 CUs)</t>
+  </si>
+  <si>
+    <t>Google 
+(40 CUs)</t>
   </si>
 </sst>
 </file>
@@ -301,7 +333,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="19">
+  <cellStyleXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -321,8 +353,20 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -336,8 +380,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="19">
+  <cellStyles count="31">
     <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="6" builtinId="9" hidden="1"/>
@@ -347,6 +394,12 @@
     <cellStyle name="Besuchter Link" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="30" builtinId="9" hidden="1"/>
     <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="5" builtinId="8" hidden="1"/>
@@ -356,9 +409,48 @@
     <cellStyle name="Link" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="29" builtinId="8" hidden="1"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="12">
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="0.0"/>
     </dxf>
@@ -418,35 +510,47 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'1 CU'!$O$18:$O$20</c:f>
+              <c:f>'1 CU'!$N$18:$N$22</c:f>
               <c:strCache>
-                <c:ptCount val="3"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>ec2+ssh://aws.amazon.com/</c:v>
+                  <c:v>FutureGrid</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>euca://india.futuregrid.org</c:v>
+                  <c:v>Amazon</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>gce+ssh://google.com</c:v>
+                  <c:v>Google</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Amazon_x000d_(40 CUs)</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Google _x000d_(40 CUs)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'1 CU'!$P$18:$P$20</c:f>
+              <c:f>'1 CU'!$P$18:$P$22</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>220.7107000827</c:v>
+                  <c:v>21.72547779082</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>21.72547779082</c:v>
+                  <c:v>220.7107000827</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>791.47931707025</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>202.2968391658</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1929.87040639</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -477,35 +581,47 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'1 CU'!$O$18:$O$20</c:f>
+              <c:f>'1 CU'!$N$18:$N$22</c:f>
               <c:strCache>
-                <c:ptCount val="3"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>ec2+ssh://aws.amazon.com/</c:v>
+                  <c:v>FutureGrid</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>euca://india.futuregrid.org</c:v>
+                  <c:v>Amazon</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>gce+ssh://google.com</c:v>
+                  <c:v>Google</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Amazon_x000d_(40 CUs)</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Google _x000d_(40 CUs)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'1 CU'!$Q$18:$Q$20</c:f>
+              <c:f>'1 CU'!$Q$18:$Q$22</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>110.47700002196</c:v>
+                  <c:v>15.09400000574</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>15.09400000574</c:v>
+                  <c:v>110.47700002196</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>139.105000019025</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>530.2727499966</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1131.60021875125</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -539,36 +655,48 @@
             <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
-                <c:f>'1 CU'!$U$18:$U$20</c:f>
+                <c:f>'1 CU'!$U$18:$U$22</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="3"/>
+                  <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>211.5752818356191</c:v>
+                    <c:v>227.927464658313</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>227.927464658313</c:v>
+                    <c:v>211.5752818356189</c:v>
                   </c:pt>
                   <c:pt idx="2">
                     <c:v>836.5967639974622</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>164.9635304236692</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>662.5074939353295</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
             </c:plus>
             <c:minus>
               <c:numRef>
-                <c:f>'1 CU'!$U$18:$U$20</c:f>
+                <c:f>'1 CU'!$U$18:$U$22</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="3"/>
+                  <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>211.5752818356191</c:v>
+                    <c:v>227.927464658313</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>227.927464658313</c:v>
+                    <c:v>211.5752818356189</c:v>
                   </c:pt>
                   <c:pt idx="2">
                     <c:v>836.5967639974622</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>164.9635304236692</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>662.5074939353295</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -585,35 +713,47 @@
           </c:errBars>
           <c:cat>
             <c:strRef>
-              <c:f>'1 CU'!$O$18:$O$20</c:f>
+              <c:f>'1 CU'!$N$18:$N$22</c:f>
               <c:strCache>
-                <c:ptCount val="3"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>ec2+ssh://aws.amazon.com/</c:v>
+                  <c:v>FutureGrid</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>euca://india.futuregrid.org</c:v>
+                  <c:v>Amazon</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>gce+ssh://google.com</c:v>
+                  <c:v>Google</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Amazon_x000d_(40 CUs)</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Google _x000d_(40 CUs)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'1 CU'!$R$18:$R$20</c:f>
+              <c:f>'1 CU'!$R$18:$R$22</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>74.09683890343001</c:v>
+                  <c:v>302.40736880304</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>302.40736880304</c:v>
+                  <c:v>74.09683890342998</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>32.68710553645</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>88.33380212783</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>47.38763433693749</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -641,35 +781,47 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'1 CU'!$O$18:$O$20</c:f>
+              <c:f>'1 CU'!$N$18:$N$22</c:f>
               <c:strCache>
-                <c:ptCount val="3"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>ec2+ssh://aws.amazon.com/</c:v>
+                  <c:v>FutureGrid</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>euca://india.futuregrid.org</c:v>
+                  <c:v>Amazon</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>gce+ssh://google.com</c:v>
+                  <c:v>Google</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Amazon_x000d_(40 CUs)</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Google _x000d_(40 CUs)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'1 CU'!$T$18:$T$20</c:f>
+              <c:f>'1 CU'!$T$18:$T$22</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>3.2009999990462</c:v>
+                  <c:v>2.776000022888</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.776000022888</c:v>
+                  <c:v>3.2009999990462</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>2.1349999904625</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.796625009777</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.4829062491675</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -685,11 +837,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="2128509784"/>
-        <c:axId val="2128512808"/>
+        <c:axId val="2120688792"/>
+        <c:axId val="2120691848"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2128509784"/>
+        <c:axId val="2120688792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -708,7 +860,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2128512808"/>
+        <c:crossAx val="2120691848"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -716,7 +868,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2128512808"/>
+        <c:axId val="2120691848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -756,7 +908,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2128509784"/>
+        <c:crossAx val="2120688792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -797,16 +949,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>806450</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>69850</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>21</xdr:col>
-      <xdr:colOff>622300</xdr:colOff>
-      <xdr:row>62</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
+      <xdr:colOff>711200</xdr:colOff>
+      <xdr:row>76</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -829,20 +981,21 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Andre Luckow" refreshedDate="41159.818736574074" createdVersion="4" refreshedVersion="4" minRefreshableVersion="3" recordCount="56">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Andre Luckow" refreshedDate="41160.662873379631" createdVersion="4" refreshedVersion="4" minRefreshableVersion="3" recordCount="67">
   <cacheSource type="worksheet">
-    <worksheetSource ref="A1:L57" sheet="1 CU"/>
+    <worksheetSource ref="A1:L68" sheet="1 CU"/>
   </cacheSource>
   <cacheFields count="12">
     <cacheField name="Run" numFmtId="0">
       <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="0" maxValue="9"/>
     </cacheField>
     <cacheField name="PC" numFmtId="0">
-      <sharedItems count="4">
+      <sharedItems count="5">
         <s v="ec2+ssh://aws.amazon.com/"/>
         <s v="gce+ssh://google.com"/>
         <s v="euca://india.futuregrid.org"/>
-        <s v="gce+ssh://google.com (multi cu)"/>
+        <s v="Google (Multi CU)"/>
+        <s v="Amazon (Multi CU)"/>
       </sharedItems>
     </cacheField>
     <cacheField name="PD" numFmtId="0">
@@ -876,10 +1029,9 @@
       <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="7.1093659396300382" maxValue="1395.8635980072499"/>
     </cacheField>
     <cacheField name="Remark" numFmtId="0">
-      <sharedItems count="3">
+      <sharedItems count="2">
         <s v="/dev/zero"/>
         <s v="/dev/urandom"/>
-        <s v="/dev/random" u="1"/>
       </sharedItems>
     </cacheField>
   </cacheFields>
@@ -892,7 +1044,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="56">
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="67">
   <r>
     <n v="0"/>
     <x v="0"/>
@@ -1677,19 +1829,174 @@
     <n v="1000.7751201542096"/>
     <x v="1"/>
   </r>
+  <r>
+    <n v="7"/>
+    <x v="3"/>
+    <s v="gs://pilot-data-cf5d0c50-f8c2-11e1-b0ff-00215ec9e3ac"/>
+    <n v="40"/>
+    <x v="0"/>
+    <n v="1968.0598649999999"/>
+    <n v="47.014433860799997"/>
+    <n v="4154.5585520300001"/>
+    <n v="1104.00799998"/>
+    <n v="3.25124998689"/>
+    <n v="1032.2250032023103"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="0"/>
+    <x v="4"/>
+    <s v="s3://pilot-data-a84f6250-f99b-11e1-818a-02215ecdd90b"/>
+    <n v="40"/>
+    <x v="0"/>
+    <n v="157.879931927"/>
+    <n v="59.8729500771"/>
+    <n v="1262.1418469"/>
+    <n v="465.93199999299998"/>
+    <n v="5.4545000255099998"/>
+    <n v="573.00246487739003"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="1"/>
+    <x v="4"/>
+    <s v="s3://pilot-data-a84f6250-f99b-11e1-818a-02215ecdd90b"/>
+    <n v="40"/>
+    <x v="0"/>
+    <n v="167.587552071"/>
+    <n v="93.305170059199995"/>
+    <n v="1325.52337098"/>
+    <n v="480.34525001600002"/>
+    <n v="6.1112500011900002"/>
+    <n v="578.17414883260994"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="2"/>
+    <x v="4"/>
+    <s v="s3://pilot-data-a84f6250-f99b-11e1-818a-02215ecdd90b"/>
+    <n v="40"/>
+    <x v="0"/>
+    <n v="333.38520407700003"/>
+    <n v="81.887583970999998"/>
+    <n v="1521.82496309"/>
+    <n v="549.14025000300001"/>
+    <n v="5.9302499949899996"/>
+    <n v="551.48167504400988"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="3"/>
+    <x v="4"/>
+    <s v="s3://pilot-data-a84f6250-f99b-11e1-818a-02215ecdd90b"/>
+    <n v="40"/>
+    <x v="0"/>
+    <n v="160.991422892"/>
+    <n v="99.748240947699998"/>
+    <n v="1164.8700099"/>
+    <n v="453.257999998"/>
+    <n v="10.2109999955"/>
+    <n v="440.66134606680009"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="4"/>
+    <x v="4"/>
+    <s v="s3://pilot-data-a84f6250-f99b-11e1-818a-02215ecdd90b"/>
+    <n v="40"/>
+    <x v="0"/>
+    <n v="367.39415502499998"/>
+    <n v="82.062947034800004"/>
+    <n v="1349.5291480999999"/>
+    <n v="442.01149998900001"/>
+    <n v="5.60025001168"/>
+    <n v="452.4602960395199"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="5"/>
+    <x v="4"/>
+    <s v="s3://pilot-data-a84f6250-f99b-11e1-818a-02215ecdd90b"/>
+    <n v="40"/>
+    <x v="0"/>
+    <n v="162.182951927"/>
+    <n v="93.295397043199998"/>
+    <n v="1511.1965069800001"/>
+    <n v="691.81049998399999"/>
+    <n v="3.8915000200300001"/>
+    <n v="560.01615800577019"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="6"/>
+    <x v="4"/>
+    <s v="s3://pilot-data-a84f6250-f99b-11e1-818a-02215ecdd90b"/>
+    <n v="40"/>
+    <x v="0"/>
+    <n v="165.01680493399999"/>
+    <n v="91.365287065499999"/>
+    <n v="1431.0721168499999"/>
+    <n v="655.00049999999999"/>
+    <n v="5.1365000188399996"/>
+    <n v="514.55302483165997"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="7"/>
+    <x v="4"/>
+    <s v="s3://pilot-data-a84f6250-f99b-11e1-818a-02215ecdd90b"/>
+    <n v="40"/>
+    <x v="0"/>
+    <n v="173.91448092499999"/>
+    <n v="95.688024997699998"/>
+    <n v="1016.85612583"/>
+    <n v="360.02674998600003"/>
+    <n v="5.0845000147799997"/>
+    <n v="382.14236990651989"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="8"/>
+    <x v="4"/>
+    <s v="s3://pilot-data-a84f6250-f99b-11e1-818a-02215ecdd90b"/>
+    <n v="40"/>
+    <x v="0"/>
+    <n v="170.93446493100001"/>
+    <n v="94.859182119400003"/>
+    <n v="1308.35150099"/>
+    <n v="507.67774998499999"/>
+    <n v="4.0910000264599997"/>
+    <n v="530.78910392813987"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="9"/>
+    <x v="4"/>
+    <s v="s3://pilot-data-a84f6250-f99b-11e1-818a-02215ecdd90b"/>
+    <n v="40"/>
+    <x v="0"/>
+    <n v="163.68142294899999"/>
+    <n v="91.253237962699998"/>
+    <n v="1518.34534502"/>
+    <n v="697.52500001199996"/>
+    <n v="6.4554999887899998"/>
+    <n v="559.43018410750994"/>
+    <x v="1"/>
+  </r>
 </pivotCacheRecords>
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0" rowHeaderCaption="">
-  <location ref="O16:U22" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="2" colPageCount="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" rowHeaderCaption="" fieldListSortAscending="1">
+  <location ref="O16:U23" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="2" colPageCount="1"/>
   <pivotFields count="12">
     <pivotField showAll="0"/>
-    <pivotField axis="axisRow" showAll="0" sortType="ascending">
-      <items count="5">
+    <pivotField axis="axisRow" showAll="0">
+      <items count="6">
+        <item x="2"/>
         <item x="0"/>
-        <item x="2"/>
         <item x="1"/>
+        <item x="4"/>
         <item x="3"/>
         <item t="default"/>
       </items>
@@ -1710,17 +2017,16 @@
     <pivotField dataField="1" numFmtId="164" showAll="0" defaultSubtotal="0"/>
     <pivotField numFmtId="164" showAll="0" defaultSubtotal="0"/>
     <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0" defaultSubtotal="0">
-      <items count="3">
+      <items count="2">
         <item x="1"/>
         <item h="1" x="0"/>
-        <item h="1" m="1" x="2"/>
       </items>
     </pivotField>
   </pivotFields>
   <rowFields count="1">
     <field x="1"/>
   </rowFields>
-  <rowItems count="5">
+  <rowItems count="6">
     <i>
       <x/>
     </i>
@@ -1732,6 +2038,9 @@
     </i>
     <i>
       <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
     </i>
     <i t="grand">
       <x/>
@@ -1773,7 +2082,7 @@
     <dataField name="STABW - Total Runtime" fld="7" subtotal="stdDev" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="1">
-    <format dxfId="0">
+    <format dxfId="11">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
   </formats>
@@ -1787,14 +2096,22 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pd_random" connectionId="2" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pd_multi_cu_1" connectionId="2" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pd" connectionId="3" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pd" connectionId="4" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pd_random" connectionId="3" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pd_multi_cu_1" connectionId="2" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pd_multi_cu" connectionId="1" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
@@ -2121,10 +2438,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1:W57"/>
+  <dimension ref="A1:V68"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T72" sqref="T72"/>
+    <sheetView tabSelected="1" topLeftCell="D12" workbookViewId="0">
+      <selection activeCell="Y47" sqref="Y47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2137,7 +2454,8 @@
     <col min="6" max="8" width="12.1640625" customWidth="1"/>
     <col min="9" max="10" width="12.1640625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12.1640625" style="8" customWidth="1"/>
-    <col min="15" max="15" width="27.33203125" customWidth="1"/>
+    <col min="14" max="14" width="16.5" customWidth="1"/>
+    <col min="15" max="15" width="24.6640625" customWidth="1"/>
     <col min="16" max="16" width="23.83203125" customWidth="1"/>
     <col min="17" max="17" width="27" customWidth="1"/>
     <col min="18" max="18" width="11.1640625" customWidth="1"/>
@@ -2784,7 +3102,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:23">
+    <row r="17" spans="1:22">
       <c r="A17">
         <v>2</v>
       </c>
@@ -2844,7 +3162,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="1:23">
+    <row r="18" spans="1:22">
       <c r="A18">
         <v>2</v>
       </c>
@@ -2883,31 +3201,34 @@
         <v>23</v>
       </c>
       <c r="N18" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="O18" s="4" t="s">
-        <v>7</v>
+        <v>37</v>
       </c>
       <c r="P18" s="5">
-        <v>220.71070008269999</v>
+        <v>21.725477790820001</v>
       </c>
       <c r="Q18" s="5">
-        <v>110.47700002196</v>
+        <v>15.09400000574</v>
       </c>
       <c r="R18" s="5">
-        <v>74.096838903430012</v>
+        <v>302.40736880303996</v>
       </c>
       <c r="S18" s="5">
-        <v>417.11351168160002</v>
+        <v>350.38976254479996</v>
       </c>
       <c r="T18" s="5">
-        <v>3.2009999990461999</v>
+        <v>2.7760000228879997</v>
       </c>
       <c r="U18" s="5">
-        <v>211.57528183561908</v>
-      </c>
-    </row>
-    <row r="19" spans="1:23">
+        <v>227.92746465831291</v>
+      </c>
+      <c r="V18" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:22">
       <c r="A19">
         <v>3</v>
       </c>
@@ -2946,35 +3267,34 @@
         <v>23</v>
       </c>
       <c r="N19" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="O19" s="4" t="s">
-        <v>37</v>
+        <v>7</v>
       </c>
       <c r="P19" s="5">
-        <v>21.725477790820001</v>
+        <v>220.71070008269999</v>
       </c>
       <c r="Q19" s="5">
-        <v>15.09400000574</v>
+        <v>110.47700002196</v>
       </c>
       <c r="R19" s="5">
-        <v>302.40736880303996</v>
+        <v>74.096838903429983</v>
       </c>
       <c r="S19" s="5">
-        <v>350.38976254479996</v>
+        <v>417.11351168160002</v>
       </c>
       <c r="T19" s="5">
-        <v>2.7760000228879997</v>
+        <v>3.2009999990461999</v>
       </c>
       <c r="U19" s="5">
-        <v>227.92746465831291</v>
-      </c>
-      <c r="W19">
-        <f>P19/P18</f>
-        <v>9.8434184580446241E-2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:23">
+        <v>211.57528183561894</v>
+      </c>
+      <c r="V19" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:22">
       <c r="A20">
         <v>3</v>
       </c>
@@ -3036,8 +3356,11 @@
       <c r="U20" s="5">
         <v>836.59676399746229</v>
       </c>
-    </row>
-    <row r="21" spans="1:23">
+      <c r="V20" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:22" ht="30">
       <c r="A21">
         <v>4</v>
       </c>
@@ -3075,29 +3398,35 @@
       <c r="L21" t="s">
         <v>23</v>
       </c>
+      <c r="N21" s="11" t="s">
+        <v>50</v>
+      </c>
       <c r="O21" s="4" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="P21" s="5">
-        <v>1924.4147694457145</v>
+        <v>202.29683916580001</v>
       </c>
       <c r="Q21" s="5">
-        <v>1135.5419642900001</v>
+        <v>530.27274999660006</v>
       </c>
       <c r="R21" s="5">
-        <v>47.440948690671426</v>
+        <v>88.333802127829998</v>
       </c>
       <c r="S21" s="5">
-        <v>4178.323398998572</v>
+        <v>1340.971093464</v>
       </c>
       <c r="T21" s="5">
-        <v>3.5160000009214287</v>
+        <v>5.7966250097770002</v>
       </c>
       <c r="U21" s="5">
-        <v>715.53232918875892</v>
-      </c>
-    </row>
-    <row r="22" spans="1:23">
+        <v>164.9635304236692</v>
+      </c>
+      <c r="V21" s="5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:22" ht="30">
       <c r="A22">
         <v>4</v>
       </c>
@@ -3135,29 +3464,35 @@
       <c r="L22" t="s">
         <v>23</v>
       </c>
+      <c r="N22" s="11" t="s">
+        <v>51</v>
+      </c>
       <c r="O22" s="4" t="s">
-        <v>17</v>
+        <v>48</v>
       </c>
       <c r="P22" s="5">
-        <v>728.94442477623465</v>
+        <v>1929.87040639</v>
       </c>
       <c r="Q22" s="5">
-        <v>372.51745193670774</v>
+        <v>1131.6002187512499</v>
       </c>
       <c r="R22" s="5">
-        <v>104.45539600115386</v>
+        <v>47.387634336937495</v>
       </c>
       <c r="S22" s="5">
-        <v>1504.1136124773843</v>
+        <v>4175.3527931275003</v>
       </c>
       <c r="T22" s="5">
-        <v>3.0400769258923837</v>
+        <v>3.4829062491675002</v>
       </c>
       <c r="U22" s="5">
-        <v>1736.6132116477979</v>
-      </c>
-    </row>
-    <row r="23" spans="1:23">
+        <v>662.50749393532953</v>
+      </c>
+      <c r="V22" s="5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:22">
       <c r="A23">
         <v>5</v>
       </c>
@@ -3195,8 +3530,29 @@
       <c r="L23" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="24" spans="1:23">
+      <c r="O23" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="P23" s="5">
+        <v>620.09684596865134</v>
+      </c>
+      <c r="Q23" s="5">
+        <v>434.92403379190273</v>
+      </c>
+      <c r="R23" s="5">
+        <v>98.545750031597308</v>
+      </c>
+      <c r="S23" s="5">
+        <v>1531.654686786</v>
+      </c>
+      <c r="T23" s="5">
+        <v>3.7907973015638374</v>
+      </c>
+      <c r="U23" s="5">
+        <v>1517.5226628650964</v>
+      </c>
+    </row>
+    <row r="24" spans="1:22">
       <c r="A24">
         <v>5</v>
       </c>
@@ -3235,7 +3591,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:23">
+    <row r="25" spans="1:22">
       <c r="A25">
         <v>6</v>
       </c>
@@ -3274,7 +3630,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:23">
+    <row r="26" spans="1:22">
       <c r="A26">
         <v>6</v>
       </c>
@@ -3313,7 +3669,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="27" spans="1:23">
+    <row r="27" spans="1:22">
       <c r="A27">
         <v>7</v>
       </c>
@@ -3352,7 +3708,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="28" spans="1:23">
+    <row r="28" spans="1:22">
       <c r="A28">
         <v>7</v>
       </c>
@@ -3391,7 +3747,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="29" spans="1:23">
+    <row r="29" spans="1:22">
       <c r="A29">
         <v>8</v>
       </c>
@@ -3430,7 +3786,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="30" spans="1:23">
+    <row r="30" spans="1:22">
       <c r="A30">
         <v>8</v>
       </c>
@@ -3469,7 +3825,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="31" spans="1:23">
+    <row r="31" spans="1:22">
       <c r="A31">
         <v>9</v>
       </c>
@@ -3508,7 +3864,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="32" spans="1:23">
+    <row r="32" spans="1:22">
       <c r="A32">
         <v>0</v>
       </c>
@@ -4086,7 +4442,7 @@
         <v>3.92000007629</v>
       </c>
       <c r="K46" s="7">
-        <f t="shared" ref="K46:K50" si="1">H46-(SUM(F46,G46,I46,J46))</f>
+        <f t="shared" ref="K46:K68" si="1">H46-(SUM(F46,G46,I46,J46))</f>
         <v>8.7560269836099991</v>
       </c>
       <c r="L46" t="s">
@@ -4250,38 +4606,38 @@
       </c>
     </row>
     <row r="51" spans="1:12">
-      <c r="A51">
+      <c r="A51" s="9">
         <v>0</v>
       </c>
-      <c r="B51" t="s">
-        <v>47</v>
-      </c>
-      <c r="C51" t="s">
+      <c r="B51" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="C51" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="D51">
+      <c r="D51" s="9">
         <v>40</v>
       </c>
-      <c r="E51">
-        <v>1024</v>
-      </c>
-      <c r="F51">
+      <c r="E51" s="9">
+        <v>1024</v>
+      </c>
+      <c r="F51" s="9">
         <v>3292.7151110200002</v>
       </c>
-      <c r="G51">
+      <c r="G51" s="9">
         <v>49.669698953599998</v>
       </c>
-      <c r="H51">
+      <c r="H51" s="9">
         <v>5451.5510759400004</v>
       </c>
-      <c r="I51">
+      <c r="I51" s="9">
         <v>1102.5932499999999</v>
       </c>
-      <c r="J51">
+      <c r="J51" s="9">
         <v>3.36800001264</v>
       </c>
       <c r="K51" s="7">
-        <f t="shared" ref="K51:K57" si="2">H51-(SUM(F51,G51,I51,J51))</f>
+        <f t="shared" si="1"/>
         <v>1003.2050159537603</v>
       </c>
       <c r="L51" t="s">
@@ -4289,38 +4645,38 @@
       </c>
     </row>
     <row r="52" spans="1:12">
-      <c r="A52">
-        <v>1</v>
-      </c>
-      <c r="B52" t="s">
-        <v>47</v>
-      </c>
-      <c r="C52" t="s">
+      <c r="A52" s="9">
+        <v>1</v>
+      </c>
+      <c r="B52" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="C52" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="D52">
+      <c r="D52" s="9">
         <v>40</v>
       </c>
-      <c r="E52">
-        <v>1024</v>
-      </c>
-      <c r="F52">
+      <c r="E52" s="9">
+        <v>1024</v>
+      </c>
+      <c r="F52" s="9">
         <v>1510.60332608</v>
       </c>
-      <c r="G52">
+      <c r="G52" s="9">
         <v>49.387537002599998</v>
       </c>
-      <c r="H52">
+      <c r="H52" s="9">
         <v>3526.6359269599998</v>
       </c>
-      <c r="I52">
+      <c r="I52" s="9">
         <v>1031.83825</v>
       </c>
-      <c r="J52">
+      <c r="J52" s="9">
         <v>2.8239999949899999</v>
       </c>
       <c r="K52" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>931.98281388240957</v>
       </c>
       <c r="L52" t="s">
@@ -4328,38 +4684,38 @@
       </c>
     </row>
     <row r="53" spans="1:12">
-      <c r="A53">
+      <c r="A53" s="9">
         <v>2</v>
       </c>
-      <c r="B53" t="s">
-        <v>47</v>
-      </c>
-      <c r="C53" t="s">
+      <c r="B53" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="C53" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="D53">
+      <c r="D53" s="9">
         <v>40</v>
       </c>
-      <c r="E53">
-        <v>1024</v>
-      </c>
-      <c r="F53">
+      <c r="E53" s="9">
+        <v>1024</v>
+      </c>
+      <c r="F53" s="9">
         <v>1709.7597661</v>
       </c>
-      <c r="G53">
+      <c r="G53" s="9">
         <v>43.468255042999999</v>
       </c>
-      <c r="H53">
+      <c r="H53" s="9">
         <v>3920.4964511399999</v>
       </c>
-      <c r="I53">
+      <c r="I53" s="9">
         <v>1122.9845</v>
       </c>
-      <c r="J53">
+      <c r="J53" s="9">
         <v>3.15425001383</v>
       </c>
       <c r="K53" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>1041.1296799831698</v>
       </c>
       <c r="L53" t="s">
@@ -4367,38 +4723,38 @@
       </c>
     </row>
     <row r="54" spans="1:12">
-      <c r="A54">
+      <c r="A54" s="9">
         <v>3</v>
       </c>
-      <c r="B54" t="s">
-        <v>47</v>
-      </c>
-      <c r="C54" t="s">
+      <c r="B54" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="C54" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="D54">
+      <c r="D54" s="9">
         <v>40</v>
       </c>
-      <c r="E54">
-        <v>1024</v>
-      </c>
-      <c r="F54">
+      <c r="E54" s="9">
+        <v>1024</v>
+      </c>
+      <c r="F54" s="9">
         <v>2592.2150978999998</v>
       </c>
-      <c r="G54">
+      <c r="G54" s="9">
         <v>49.294908046700002</v>
       </c>
-      <c r="H54">
+      <c r="H54" s="9">
         <v>4692.7860889399999</v>
       </c>
-      <c r="I54">
+      <c r="I54" s="9">
         <v>1036.7059999999999</v>
       </c>
-      <c r="J54">
+      <c r="J54" s="9">
         <v>3.1137499928499999</v>
       </c>
       <c r="K54" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>1011.4563330004503</v>
       </c>
       <c r="L54" t="s">
@@ -4406,38 +4762,38 @@
       </c>
     </row>
     <row r="55" spans="1:12">
-      <c r="A55">
+      <c r="A55" s="9">
         <v>4</v>
       </c>
-      <c r="B55" t="s">
-        <v>47</v>
-      </c>
-      <c r="C55" t="s">
+      <c r="B55" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="C55" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="D55">
+      <c r="D55" s="9">
         <v>40</v>
       </c>
-      <c r="E55">
-        <v>1024</v>
-      </c>
-      <c r="F55">
+      <c r="E55" s="9">
+        <v>1024</v>
+      </c>
+      <c r="F55" s="9">
         <v>1849.0491790799999</v>
       </c>
-      <c r="G55">
+      <c r="G55" s="9">
         <v>46.814173936800003</v>
       </c>
-      <c r="H55">
+      <c r="H55" s="9">
         <v>4417.4567010399996</v>
       </c>
-      <c r="I55">
+      <c r="I55" s="9">
         <v>1122.83800002</v>
       </c>
-      <c r="J55">
+      <c r="J55" s="9">
         <v>2.8917499959500002</v>
       </c>
       <c r="K55" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>1395.8635980072499</v>
       </c>
       <c r="L55" t="s">
@@ -4445,38 +4801,38 @@
       </c>
     </row>
     <row r="56" spans="1:12">
-      <c r="A56">
+      <c r="A56" s="9">
         <v>5</v>
       </c>
-      <c r="B56" t="s">
-        <v>47</v>
-      </c>
-      <c r="C56" t="s">
+      <c r="B56" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="C56" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="D56">
+      <c r="D56" s="9">
         <v>40</v>
       </c>
-      <c r="E56">
-        <v>1024</v>
-      </c>
-      <c r="F56">
+      <c r="E56" s="9">
+        <v>1024</v>
+      </c>
+      <c r="F56" s="9">
         <v>1105.9794080300001</v>
       </c>
-      <c r="G56">
+      <c r="G56" s="9">
         <v>46.863272905300001</v>
       </c>
-      <c r="H56">
+      <c r="H56" s="9">
         <v>3702.10813594</v>
       </c>
-      <c r="I56">
+      <c r="I56" s="9">
         <v>1459.53800002</v>
       </c>
-      <c r="J56">
+      <c r="J56" s="9">
         <v>2.2719999671000002</v>
       </c>
       <c r="K56" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>1087.4554550176003</v>
       </c>
       <c r="L56" t="s">
@@ -4487,8 +4843,8 @@
       <c r="A57">
         <v>6</v>
       </c>
-      <c r="B57" t="s">
-        <v>47</v>
+      <c r="B57" s="9" t="s">
+        <v>48</v>
       </c>
       <c r="C57" t="s">
         <v>42</v>
@@ -4515,10 +4871,439 @@
         <v>6.9882500290899996</v>
       </c>
       <c r="K57" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>1000.7751201542096</v>
       </c>
       <c r="L57" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12">
+      <c r="A58">
+        <v>7</v>
+      </c>
+      <c r="B58" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="C58" t="s">
+        <v>42</v>
+      </c>
+      <c r="D58">
+        <v>40</v>
+      </c>
+      <c r="E58">
+        <v>1024</v>
+      </c>
+      <c r="F58">
+        <v>1968.0598649999999</v>
+      </c>
+      <c r="G58">
+        <v>47.014433860799997</v>
+      </c>
+      <c r="H58">
+        <v>4154.5585520300001</v>
+      </c>
+      <c r="I58">
+        <v>1104.00799998</v>
+      </c>
+      <c r="J58">
+        <v>3.25124998689</v>
+      </c>
+      <c r="K58" s="7">
+        <f t="shared" si="1"/>
+        <v>1032.2250032023103</v>
+      </c>
+      <c r="L58" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12">
+      <c r="A59">
+        <v>0</v>
+      </c>
+      <c r="B59" t="s">
+        <v>49</v>
+      </c>
+      <c r="C59" t="s">
+        <v>47</v>
+      </c>
+      <c r="D59">
+        <v>40</v>
+      </c>
+      <c r="E59">
+        <v>1024</v>
+      </c>
+      <c r="F59">
+        <v>157.879931927</v>
+      </c>
+      <c r="G59">
+        <v>59.8729500771</v>
+      </c>
+      <c r="H59">
+        <v>1262.1418469</v>
+      </c>
+      <c r="I59">
+        <v>465.93199999299998</v>
+      </c>
+      <c r="J59">
+        <v>5.4545000255099998</v>
+      </c>
+      <c r="K59" s="7">
+        <f t="shared" si="1"/>
+        <v>573.00246487739003</v>
+      </c>
+      <c r="L59" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12">
+      <c r="A60">
+        <v>1</v>
+      </c>
+      <c r="B60" t="s">
+        <v>49</v>
+      </c>
+      <c r="C60" t="s">
+        <v>47</v>
+      </c>
+      <c r="D60">
+        <v>40</v>
+      </c>
+      <c r="E60">
+        <v>1024</v>
+      </c>
+      <c r="F60">
+        <v>167.587552071</v>
+      </c>
+      <c r="G60">
+        <v>93.305170059199995</v>
+      </c>
+      <c r="H60">
+        <v>1325.52337098</v>
+      </c>
+      <c r="I60">
+        <v>480.34525001600002</v>
+      </c>
+      <c r="J60">
+        <v>6.1112500011900002</v>
+      </c>
+      <c r="K60" s="7">
+        <f t="shared" si="1"/>
+        <v>578.17414883260994</v>
+      </c>
+      <c r="L60" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12">
+      <c r="A61">
+        <v>2</v>
+      </c>
+      <c r="B61" t="s">
+        <v>49</v>
+      </c>
+      <c r="C61" t="s">
+        <v>47</v>
+      </c>
+      <c r="D61">
+        <v>40</v>
+      </c>
+      <c r="E61">
+        <v>1024</v>
+      </c>
+      <c r="F61">
+        <v>333.38520407700003</v>
+      </c>
+      <c r="G61">
+        <v>81.887583970999998</v>
+      </c>
+      <c r="H61">
+        <v>1521.82496309</v>
+      </c>
+      <c r="I61">
+        <v>549.14025000300001</v>
+      </c>
+      <c r="J61">
+        <v>5.9302499949899996</v>
+      </c>
+      <c r="K61" s="7">
+        <f t="shared" si="1"/>
+        <v>551.48167504400988</v>
+      </c>
+      <c r="L61" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12">
+      <c r="A62">
+        <v>3</v>
+      </c>
+      <c r="B62" t="s">
+        <v>49</v>
+      </c>
+      <c r="C62" t="s">
+        <v>47</v>
+      </c>
+      <c r="D62">
+        <v>40</v>
+      </c>
+      <c r="E62">
+        <v>1024</v>
+      </c>
+      <c r="F62">
+        <v>160.991422892</v>
+      </c>
+      <c r="G62">
+        <v>99.748240947699998</v>
+      </c>
+      <c r="H62">
+        <v>1164.8700099</v>
+      </c>
+      <c r="I62">
+        <v>453.257999998</v>
+      </c>
+      <c r="J62">
+        <v>10.2109999955</v>
+      </c>
+      <c r="K62" s="7">
+        <f t="shared" si="1"/>
+        <v>440.66134606680009</v>
+      </c>
+      <c r="L62" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12">
+      <c r="A63">
+        <v>4</v>
+      </c>
+      <c r="B63" t="s">
+        <v>49</v>
+      </c>
+      <c r="C63" t="s">
+        <v>47</v>
+      </c>
+      <c r="D63">
+        <v>40</v>
+      </c>
+      <c r="E63">
+        <v>1024</v>
+      </c>
+      <c r="F63">
+        <v>367.39415502499998</v>
+      </c>
+      <c r="G63">
+        <v>82.062947034800004</v>
+      </c>
+      <c r="H63">
+        <v>1349.5291480999999</v>
+      </c>
+      <c r="I63">
+        <v>442.01149998900001</v>
+      </c>
+      <c r="J63">
+        <v>5.60025001168</v>
+      </c>
+      <c r="K63" s="7">
+        <f t="shared" si="1"/>
+        <v>452.4602960395199</v>
+      </c>
+      <c r="L63" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12">
+      <c r="A64">
+        <v>5</v>
+      </c>
+      <c r="B64" t="s">
+        <v>49</v>
+      </c>
+      <c r="C64" t="s">
+        <v>47</v>
+      </c>
+      <c r="D64">
+        <v>40</v>
+      </c>
+      <c r="E64">
+        <v>1024</v>
+      </c>
+      <c r="F64">
+        <v>162.182951927</v>
+      </c>
+      <c r="G64">
+        <v>93.295397043199998</v>
+      </c>
+      <c r="H64">
+        <v>1511.1965069800001</v>
+      </c>
+      <c r="I64">
+        <v>691.81049998399999</v>
+      </c>
+      <c r="J64">
+        <v>3.8915000200300001</v>
+      </c>
+      <c r="K64" s="7">
+        <f t="shared" si="1"/>
+        <v>560.01615800577019</v>
+      </c>
+      <c r="L64" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12">
+      <c r="A65">
+        <v>6</v>
+      </c>
+      <c r="B65" t="s">
+        <v>49</v>
+      </c>
+      <c r="C65" t="s">
+        <v>47</v>
+      </c>
+      <c r="D65">
+        <v>40</v>
+      </c>
+      <c r="E65">
+        <v>1024</v>
+      </c>
+      <c r="F65">
+        <v>165.01680493399999</v>
+      </c>
+      <c r="G65">
+        <v>91.365287065499999</v>
+      </c>
+      <c r="H65">
+        <v>1431.0721168499999</v>
+      </c>
+      <c r="I65">
+        <v>655.00049999999999</v>
+      </c>
+      <c r="J65">
+        <v>5.1365000188399996</v>
+      </c>
+      <c r="K65" s="7">
+        <f t="shared" si="1"/>
+        <v>514.55302483165997</v>
+      </c>
+      <c r="L65" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12">
+      <c r="A66">
+        <v>7</v>
+      </c>
+      <c r="B66" t="s">
+        <v>49</v>
+      </c>
+      <c r="C66" t="s">
+        <v>47</v>
+      </c>
+      <c r="D66">
+        <v>40</v>
+      </c>
+      <c r="E66">
+        <v>1024</v>
+      </c>
+      <c r="F66">
+        <v>173.91448092499999</v>
+      </c>
+      <c r="G66">
+        <v>95.688024997699998</v>
+      </c>
+      <c r="H66">
+        <v>1016.85612583</v>
+      </c>
+      <c r="I66">
+        <v>360.02674998600003</v>
+      </c>
+      <c r="J66">
+        <v>5.0845000147799997</v>
+      </c>
+      <c r="K66" s="7">
+        <f t="shared" si="1"/>
+        <v>382.14236990651989</v>
+      </c>
+      <c r="L66" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12">
+      <c r="A67">
+        <v>8</v>
+      </c>
+      <c r="B67" t="s">
+        <v>49</v>
+      </c>
+      <c r="C67" t="s">
+        <v>47</v>
+      </c>
+      <c r="D67">
+        <v>40</v>
+      </c>
+      <c r="E67">
+        <v>1024</v>
+      </c>
+      <c r="F67">
+        <v>170.93446493100001</v>
+      </c>
+      <c r="G67">
+        <v>94.859182119400003</v>
+      </c>
+      <c r="H67">
+        <v>1308.35150099</v>
+      </c>
+      <c r="I67">
+        <v>507.67774998499999</v>
+      </c>
+      <c r="J67">
+        <v>4.0910000264599997</v>
+      </c>
+      <c r="K67" s="7">
+        <f t="shared" si="1"/>
+        <v>530.78910392813987</v>
+      </c>
+      <c r="L67" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12">
+      <c r="A68">
+        <v>9</v>
+      </c>
+      <c r="B68" t="s">
+        <v>49</v>
+      </c>
+      <c r="C68" t="s">
+        <v>47</v>
+      </c>
+      <c r="D68">
+        <v>40</v>
+      </c>
+      <c r="E68">
+        <v>1024</v>
+      </c>
+      <c r="F68">
+        <v>163.68142294899999</v>
+      </c>
+      <c r="G68">
+        <v>91.253237962699998</v>
+      </c>
+      <c r="H68">
+        <v>1518.34534502</v>
+      </c>
+      <c r="I68">
+        <v>697.52500001199996</v>
+      </c>
+      <c r="J68">
+        <v>6.4554999887899998</v>
+      </c>
+      <c r="K68" s="7">
+        <f t="shared" si="1"/>
+        <v>559.43018410750994</v>
+      </c>
+      <c r="L68" t="s">
         <v>31</v>
       </c>
     </row>
@@ -4530,6 +5315,9 @@
       </customFilters>
     </filterColumn>
   </autoFilter>
+  <sortState ref="O16:U23">
+    <sortCondition ref="Q18"/>
+  </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId2"/>
@@ -4543,16 +5331,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L11"/>
+  <dimension ref="A1:L22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:L11"/>
+      <selection activeCell="A2" sqref="A2:J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="4.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="47.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="5.1640625" bestFit="1" customWidth="1"/>
@@ -4617,19 +5405,19 @@
         <v>1024</v>
       </c>
       <c r="F2" s="9">
-        <v>803.12535190000006</v>
+        <v>803.12535190599999</v>
       </c>
       <c r="G2" s="9">
-        <v>50.412962909999997</v>
+        <v>50.412962913500003</v>
       </c>
       <c r="H2" s="9">
-        <v>1258.991186</v>
+        <v>1258.9911858999999</v>
       </c>
       <c r="I2" s="9">
-        <v>224.01374999999999</v>
+        <v>224.01374998700001</v>
       </c>
       <c r="J2" s="9">
-        <v>2.7437500359999998</v>
+        <v>2.7437500357600002</v>
       </c>
       <c r="K2" s="10">
         <v>178.7</v>
@@ -4655,19 +5443,19 @@
         <v>1024</v>
       </c>
       <c r="F3" s="9">
-        <v>1014.129175</v>
+        <v>1014.12917495</v>
       </c>
       <c r="G3" s="9">
-        <v>49.989407059999998</v>
+        <v>49.9894070625</v>
       </c>
       <c r="H3" s="9">
-        <v>1427.354409</v>
+        <v>1427.35440898</v>
       </c>
       <c r="I3" s="9">
-        <v>212.36250000000001</v>
+        <v>212.362500012</v>
       </c>
       <c r="J3" s="9">
-        <v>2.8700000050000001</v>
+        <v>2.8700000047700001</v>
       </c>
       <c r="K3" s="10">
         <v>148</v>
@@ -4693,19 +5481,19 @@
         <v>1024</v>
       </c>
       <c r="F4" s="9">
-        <v>1231.611101</v>
+        <v>1231.61110091</v>
       </c>
       <c r="G4" s="9">
-        <v>48.882606029999998</v>
+        <v>48.882606029500003</v>
       </c>
       <c r="H4" s="9">
-        <v>1653.6969349999999</v>
+        <v>1653.6969349399999</v>
       </c>
       <c r="I4" s="9">
-        <v>237.79249999999999</v>
+        <v>237.79249998899999</v>
       </c>
       <c r="J4" s="9">
-        <v>2.047500044</v>
+        <v>2.04750004411</v>
       </c>
       <c r="K4" s="10">
         <v>133.4</v>
@@ -4731,19 +5519,19 @@
         <v>1024</v>
       </c>
       <c r="F5" s="9">
-        <v>3292.715111</v>
+        <v>3292.7151110200002</v>
       </c>
       <c r="G5" s="9">
-        <v>49.669698949999997</v>
+        <v>49.669698953599998</v>
       </c>
       <c r="H5" s="9">
-        <v>5451.5510759999997</v>
+        <v>5451.5510759400004</v>
       </c>
       <c r="I5" s="9">
         <v>1102.5932499999999</v>
       </c>
       <c r="J5" s="9">
-        <v>3.3680000130000001</v>
+        <v>3.36800001264</v>
       </c>
       <c r="K5" s="10">
         <v>1003.2</v>
@@ -4769,19 +5557,19 @@
         <v>1024</v>
       </c>
       <c r="F6" s="9">
-        <v>1510.6033259999999</v>
+        <v>1510.60332608</v>
       </c>
       <c r="G6" s="9">
-        <v>49.387537000000002</v>
+        <v>49.387537002599998</v>
       </c>
       <c r="H6" s="9">
-        <v>3526.6359269999998</v>
+        <v>3526.6359269599998</v>
       </c>
       <c r="I6" s="9">
         <v>1031.83825</v>
       </c>
       <c r="J6" s="9">
-        <v>2.8239999949999999</v>
+        <v>2.8239999949899999</v>
       </c>
       <c r="K6" s="10">
         <v>932</v>
@@ -4807,19 +5595,19 @@
         <v>1024</v>
       </c>
       <c r="F7" s="9">
-        <v>1709.7597659999999</v>
+        <v>1709.7597661</v>
       </c>
       <c r="G7" s="9">
-        <v>43.468255040000003</v>
+        <v>43.468255042999999</v>
       </c>
       <c r="H7" s="9">
-        <v>3920.496451</v>
+        <v>3920.4964511399999</v>
       </c>
       <c r="I7" s="9">
         <v>1122.9845</v>
       </c>
       <c r="J7" s="9">
-        <v>3.154250014</v>
+        <v>3.15425001383</v>
       </c>
       <c r="K7" s="10">
         <v>1041.0999999999999</v>
@@ -4845,19 +5633,19 @@
         <v>1024</v>
       </c>
       <c r="F8" s="9">
-        <v>2592.2150980000001</v>
+        <v>2592.2150978999998</v>
       </c>
       <c r="G8" s="9">
-        <v>49.294908049999997</v>
+        <v>49.294908046700002</v>
       </c>
       <c r="H8" s="9">
-        <v>4692.7860890000002</v>
+        <v>4692.7860889399999</v>
       </c>
       <c r="I8" s="9">
         <v>1036.7059999999999</v>
       </c>
       <c r="J8" s="9">
-        <v>3.1137499929999999</v>
+        <v>3.1137499928499999</v>
       </c>
       <c r="K8" s="10">
         <v>1011.5</v>
@@ -4883,19 +5671,19 @@
         <v>1024</v>
       </c>
       <c r="F9" s="9">
-        <v>1849.0491790000001</v>
+        <v>1849.0491790799999</v>
       </c>
       <c r="G9" s="9">
-        <v>46.814173940000003</v>
+        <v>46.814173936800003</v>
       </c>
       <c r="H9" s="9">
-        <v>4417.4567010000001</v>
+        <v>4417.4567010399996</v>
       </c>
       <c r="I9" s="9">
-        <v>1122.838</v>
+        <v>1122.83800002</v>
       </c>
       <c r="J9" s="9">
-        <v>2.8917499960000002</v>
+        <v>2.8917499959500002</v>
       </c>
       <c r="K9" s="10">
         <v>1395.9</v>
@@ -4921,19 +5709,19 @@
         <v>1024</v>
       </c>
       <c r="F10" s="9">
-        <v>1105.9794079999999</v>
+        <v>1105.9794080300001</v>
       </c>
       <c r="G10" s="9">
-        <v>46.863272909999999</v>
+        <v>46.863272905300001</v>
       </c>
       <c r="H10" s="9">
-        <v>3702.1081359999998</v>
+        <v>3702.10813594</v>
       </c>
       <c r="I10" s="9">
-        <v>1459.538</v>
+        <v>1459.53800002</v>
       </c>
       <c r="J10" s="9">
-        <v>2.2719999670000002</v>
+        <v>2.2719999671000002</v>
       </c>
       <c r="K10" s="10">
         <v>1087.5</v>
@@ -4943,40 +5731,458 @@
       </c>
     </row>
     <row r="11" spans="1:12">
-      <c r="A11" s="9">
+      <c r="A11">
         <v>6</v>
       </c>
-      <c r="B11" s="9" t="s">
+      <c r="B11" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="9" t="s">
+      <c r="C11" t="s">
         <v>42</v>
       </c>
-      <c r="D11" s="9">
+      <c r="D11">
         <v>40</v>
       </c>
-      <c r="E11" s="9">
-        <v>1024</v>
-      </c>
-      <c r="F11" s="9">
-        <v>1410.581498</v>
-      </c>
-      <c r="G11" s="9">
-        <v>46.58879495</v>
-      </c>
-      <c r="H11" s="9">
-        <v>3537.229413</v>
-      </c>
-      <c r="I11" s="9">
-        <v>1072.29575</v>
-      </c>
-      <c r="J11" s="9">
-        <v>6.9882500289999996</v>
+      <c r="E11">
+        <v>1024</v>
+      </c>
+      <c r="F11">
+        <v>1410.5814979100001</v>
+      </c>
+      <c r="G11">
+        <v>46.588794946699998</v>
+      </c>
+      <c r="H11">
+        <v>3537.2294130300002</v>
+      </c>
+      <c r="I11">
+        <v>1072.2957499900001</v>
+      </c>
+      <c r="J11">
+        <v>6.9882500290899996</v>
       </c>
       <c r="K11" s="10">
         <v>1000.8</v>
       </c>
       <c r="L11" s="9" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
+      <c r="A12">
+        <v>7</v>
+      </c>
+      <c r="B12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" t="s">
+        <v>42</v>
+      </c>
+      <c r="D12">
+        <v>40</v>
+      </c>
+      <c r="E12">
+        <v>1024</v>
+      </c>
+      <c r="F12">
+        <v>1968.0598649999999</v>
+      </c>
+      <c r="G12">
+        <v>47.014433860799997</v>
+      </c>
+      <c r="H12">
+        <v>4154.5585520300001</v>
+      </c>
+      <c r="I12">
+        <v>1104.00799998</v>
+      </c>
+      <c r="J12">
+        <v>3.25124998689</v>
+      </c>
+      <c r="K12" s="10">
+        <v>1001.8</v>
+      </c>
+      <c r="L12" s="9" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
+      <c r="A13">
+        <v>0</v>
+      </c>
+      <c r="B13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" t="s">
+        <v>47</v>
+      </c>
+      <c r="D13">
+        <v>40</v>
+      </c>
+      <c r="E13">
+        <v>1024</v>
+      </c>
+      <c r="F13">
+        <v>157.879931927</v>
+      </c>
+      <c r="G13">
+        <v>59.8729500771</v>
+      </c>
+      <c r="H13">
+        <v>1262.1418469</v>
+      </c>
+      <c r="I13">
+        <v>465.93199999299998</v>
+      </c>
+      <c r="J13">
+        <v>5.4545000255099998</v>
+      </c>
+      <c r="K13" s="10">
+        <v>1002.8</v>
+      </c>
+      <c r="L13" s="9" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12">
+      <c r="A14">
+        <v>1</v>
+      </c>
+      <c r="B14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" t="s">
+        <v>47</v>
+      </c>
+      <c r="D14">
+        <v>40</v>
+      </c>
+      <c r="E14">
+        <v>1024</v>
+      </c>
+      <c r="F14">
+        <v>167.587552071</v>
+      </c>
+      <c r="G14">
+        <v>93.305170059199995</v>
+      </c>
+      <c r="H14">
+        <v>1325.52337098</v>
+      </c>
+      <c r="I14">
+        <v>480.34525001600002</v>
+      </c>
+      <c r="J14">
+        <v>6.1112500011900002</v>
+      </c>
+      <c r="K14" s="10">
+        <v>1003.8</v>
+      </c>
+      <c r="L14" s="9" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12">
+      <c r="A15">
+        <v>2</v>
+      </c>
+      <c r="B15" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" t="s">
+        <v>47</v>
+      </c>
+      <c r="D15">
+        <v>40</v>
+      </c>
+      <c r="E15">
+        <v>1024</v>
+      </c>
+      <c r="F15">
+        <v>333.38520407700003</v>
+      </c>
+      <c r="G15">
+        <v>81.887583970999998</v>
+      </c>
+      <c r="H15">
+        <v>1521.82496309</v>
+      </c>
+      <c r="I15">
+        <v>549.14025000300001</v>
+      </c>
+      <c r="J15">
+        <v>5.9302499949899996</v>
+      </c>
+      <c r="K15" s="10">
+        <v>1004.8</v>
+      </c>
+      <c r="L15" s="9" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12">
+      <c r="A16">
+        <v>3</v>
+      </c>
+      <c r="B16" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" t="s">
+        <v>47</v>
+      </c>
+      <c r="D16">
+        <v>40</v>
+      </c>
+      <c r="E16">
+        <v>1024</v>
+      </c>
+      <c r="F16">
+        <v>160.991422892</v>
+      </c>
+      <c r="G16">
+        <v>99.748240947699998</v>
+      </c>
+      <c r="H16">
+        <v>1164.8700099</v>
+      </c>
+      <c r="I16">
+        <v>453.257999998</v>
+      </c>
+      <c r="J16">
+        <v>10.2109999955</v>
+      </c>
+      <c r="K16" s="10">
+        <v>1005.8</v>
+      </c>
+      <c r="L16" s="9" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12">
+      <c r="A17">
+        <v>4</v>
+      </c>
+      <c r="B17" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17" t="s">
+        <v>47</v>
+      </c>
+      <c r="D17">
+        <v>40</v>
+      </c>
+      <c r="E17">
+        <v>1024</v>
+      </c>
+      <c r="F17">
+        <v>367.39415502499998</v>
+      </c>
+      <c r="G17">
+        <v>82.062947034800004</v>
+      </c>
+      <c r="H17">
+        <v>1349.5291480999999</v>
+      </c>
+      <c r="I17">
+        <v>442.01149998900001</v>
+      </c>
+      <c r="J17">
+        <v>5.60025001168</v>
+      </c>
+      <c r="K17" s="10">
+        <v>1006.8</v>
+      </c>
+      <c r="L17" s="9" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12">
+      <c r="A18">
+        <v>5</v>
+      </c>
+      <c r="B18" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18" t="s">
+        <v>47</v>
+      </c>
+      <c r="D18">
+        <v>40</v>
+      </c>
+      <c r="E18">
+        <v>1024</v>
+      </c>
+      <c r="F18">
+        <v>162.182951927</v>
+      </c>
+      <c r="G18">
+        <v>93.295397043199998</v>
+      </c>
+      <c r="H18">
+        <v>1511.1965069800001</v>
+      </c>
+      <c r="I18">
+        <v>691.81049998399999</v>
+      </c>
+      <c r="J18">
+        <v>3.8915000200300001</v>
+      </c>
+      <c r="K18" s="10">
+        <v>1007.8</v>
+      </c>
+      <c r="L18" s="9" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12">
+      <c r="A19">
+        <v>6</v>
+      </c>
+      <c r="B19" t="s">
+        <v>7</v>
+      </c>
+      <c r="C19" t="s">
+        <v>47</v>
+      </c>
+      <c r="D19">
+        <v>40</v>
+      </c>
+      <c r="E19">
+        <v>1024</v>
+      </c>
+      <c r="F19">
+        <v>165.01680493399999</v>
+      </c>
+      <c r="G19">
+        <v>91.365287065499999</v>
+      </c>
+      <c r="H19">
+        <v>1431.0721168499999</v>
+      </c>
+      <c r="I19">
+        <v>655.00049999999999</v>
+      </c>
+      <c r="J19">
+        <v>5.1365000188399996</v>
+      </c>
+      <c r="K19" s="10">
+        <v>1008.8</v>
+      </c>
+      <c r="L19" s="9" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12">
+      <c r="A20">
+        <v>7</v>
+      </c>
+      <c r="B20" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20" t="s">
+        <v>47</v>
+      </c>
+      <c r="D20">
+        <v>40</v>
+      </c>
+      <c r="E20">
+        <v>1024</v>
+      </c>
+      <c r="F20">
+        <v>173.91448092499999</v>
+      </c>
+      <c r="G20">
+        <v>95.688024997699998</v>
+      </c>
+      <c r="H20">
+        <v>1016.85612583</v>
+      </c>
+      <c r="I20">
+        <v>360.02674998600003</v>
+      </c>
+      <c r="J20">
+        <v>5.0845000147799997</v>
+      </c>
+      <c r="K20" s="10">
+        <v>1009.8</v>
+      </c>
+      <c r="L20" s="9" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12">
+      <c r="A21">
+        <v>8</v>
+      </c>
+      <c r="B21" t="s">
+        <v>7</v>
+      </c>
+      <c r="C21" t="s">
+        <v>47</v>
+      </c>
+      <c r="D21">
+        <v>40</v>
+      </c>
+      <c r="E21">
+        <v>1024</v>
+      </c>
+      <c r="F21">
+        <v>170.93446493100001</v>
+      </c>
+      <c r="G21">
+        <v>94.859182119400003</v>
+      </c>
+      <c r="H21">
+        <v>1308.35150099</v>
+      </c>
+      <c r="I21">
+        <v>507.67774998499999</v>
+      </c>
+      <c r="J21">
+        <v>4.0910000264599997</v>
+      </c>
+      <c r="K21" s="10">
+        <v>1010.8</v>
+      </c>
+      <c r="L21" s="9" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12">
+      <c r="A22">
+        <v>9</v>
+      </c>
+      <c r="B22" t="s">
+        <v>7</v>
+      </c>
+      <c r="C22" t="s">
+        <v>47</v>
+      </c>
+      <c r="D22">
+        <v>40</v>
+      </c>
+      <c r="E22">
+        <v>1024</v>
+      </c>
+      <c r="F22">
+        <v>163.68142294899999</v>
+      </c>
+      <c r="G22">
+        <v>91.253237962699998</v>
+      </c>
+      <c r="H22">
+        <v>1518.34534502</v>
+      </c>
+      <c r="I22">
+        <v>697.52500001199996</v>
+      </c>
+      <c r="J22">
+        <v>6.4554999887899998</v>
+      </c>
+      <c r="K22" s="10">
+        <v>1011.8</v>
+      </c>
+      <c r="L22" s="9" t="s">
         <v>43</v>
       </c>
     </row>

</xml_diff>

<commit_message>
finished draft of performance section 6.1
git-svn-id: file://localhost/tmp/svn2git/svn@7766 defb5e50-622e-49ec-a68e-d72c7db87b45
</commit_message>
<xml_diff>
--- a/papers/ccpe-cloud12/performance/pd.xlsx
+++ b/papers/ccpe-cloud12/performance/pd.xlsx
@@ -375,25 +375,9 @@
     <t>ssh://luckow@india.futuregrid.org/tmp/pilot-data-al-b7923bce-fa9b-11e1-84f8-00215ec9e3ac</t>
   </si>
   <si>
-    <t>FG/Walrus
-(b1)</t>
-  </si>
-  <si>
-    <t>FG/SSH
-(b2)</t>
-  </si>
-  <si>
-    <t>Amazon
-(b4)</t>
-  </si>
-  <si>
     <t>Amazon 
 (Multi CUs)
 (b5)</t>
-  </si>
-  <si>
-    <t>Google 
-(b6)</t>
   </si>
   <si>
     <t>Google 
@@ -416,6 +400,26 @@
     <t>FG/Walrus
 (Multi CU)
 (b3)</t>
+  </si>
+  <si>
+    <t>FG/SSH
+(Single CU)
+(b2)</t>
+  </si>
+  <si>
+    <t>FG/Walrus
+(Single CU)
+(b1)</t>
+  </si>
+  <si>
+    <t>Amazon
+(Single CU)
+(b4)</t>
+  </si>
+  <si>
+    <t>Google
+(Single CU) 
+(b6)</t>
   </si>
 </sst>
 </file>
@@ -748,22 +752,22 @@
               <c:strCache>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>FG/Walrus_x000d_(b1)</c:v>
+                  <c:v>FG/Walrus_x000d_(Single CU)_x000d_(b1)</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>FG/SSH_x000d_(b2)</c:v>
+                  <c:v>FG/SSH_x000d_(Single CU)_x000d_(b2)</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>FG/Walrus_x000d_(Multi CU)_x000d_(b3)</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Amazon_x000d_(b4)</c:v>
+                  <c:v>Amazon_x000d_(Single CU)_x000d_(b4)</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>Amazon _x000d_(Multi CUs)_x000d_(b5)</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>Google _x000d_(b6)</c:v>
+                  <c:v>Google_x000d_(Single CU) _x000d_(b6)</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>Google _x000d_(Multi CUs)_x000d_(b7)</c:v>
@@ -831,22 +835,22 @@
               <c:strCache>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>FG/Walrus_x000d_(b1)</c:v>
+                  <c:v>FG/Walrus_x000d_(Single CU)_x000d_(b1)</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>FG/SSH_x000d_(b2)</c:v>
+                  <c:v>FG/SSH_x000d_(Single CU)_x000d_(b2)</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>FG/Walrus_x000d_(Multi CU)_x000d_(b3)</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Amazon_x000d_(b4)</c:v>
+                  <c:v>Amazon_x000d_(Single CU)_x000d_(b4)</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>Amazon _x000d_(Multi CUs)_x000d_(b5)</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>Google _x000d_(b6)</c:v>
+                  <c:v>Google_x000d_(Single CU) _x000d_(b6)</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>Google _x000d_(Multi CUs)_x000d_(b7)</c:v>
@@ -987,22 +991,22 @@
               <c:strCache>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>FG/Walrus_x000d_(b1)</c:v>
+                  <c:v>FG/Walrus_x000d_(Single CU)_x000d_(b1)</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>FG/SSH_x000d_(b2)</c:v>
+                  <c:v>FG/SSH_x000d_(Single CU)_x000d_(b2)</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>FG/Walrus_x000d_(Multi CU)_x000d_(b3)</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Amazon_x000d_(b4)</c:v>
+                  <c:v>Amazon_x000d_(Single CU)_x000d_(b4)</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>Amazon _x000d_(Multi CUs)_x000d_(b5)</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>Google _x000d_(b6)</c:v>
+                  <c:v>Google_x000d_(Single CU) _x000d_(b6)</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>Google _x000d_(Multi CUs)_x000d_(b7)</c:v>
@@ -1067,22 +1071,22 @@
               <c:strCache>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>FG/Walrus_x000d_(b1)</c:v>
+                  <c:v>FG/Walrus_x000d_(Single CU)_x000d_(b1)</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>FG/SSH_x000d_(b2)</c:v>
+                  <c:v>FG/SSH_x000d_(Single CU)_x000d_(b2)</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>FG/Walrus_x000d_(Multi CU)_x000d_(b3)</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Amazon_x000d_(b4)</c:v>
+                  <c:v>Amazon_x000d_(Single CU)_x000d_(b4)</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>Amazon _x000d_(Multi CUs)_x000d_(b5)</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>Google _x000d_(b6)</c:v>
+                  <c:v>Google_x000d_(Single CU) _x000d_(b6)</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>Google _x000d_(Multi CUs)_x000d_(b7)</c:v>
@@ -3468,8 +3472,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V110"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N20" sqref="N20"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="N23" sqref="N23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4182,7 +4186,7 @@
         <v>32</v>
       </c>
       <c r="R16" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="S16" t="s">
         <v>23</v>
@@ -4197,7 +4201,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="17" spans="1:22" ht="30">
+    <row r="17" spans="1:22" ht="45">
       <c r="A17">
         <v>3</v>
       </c>
@@ -4239,10 +4243,10 @@
         <v>4</v>
       </c>
       <c r="N17" s="11" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="O17" s="4" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="P17" s="5">
         <v>21.725477790819998</v>
@@ -4266,7 +4270,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:22" ht="30">
+    <row r="18" spans="1:22" ht="45">
       <c r="A18">
         <v>3</v>
       </c>
@@ -4308,10 +4312,10 @@
         <v>6</v>
       </c>
       <c r="N18" s="11" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="O18" s="4" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="P18" s="5">
         <v>17.954139757180002</v>
@@ -4377,7 +4381,7 @@
         <v>4</v>
       </c>
       <c r="N19" s="11" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="O19" s="4" t="s">
         <v>57</v>
@@ -4404,7 +4408,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:22" ht="30">
+    <row r="20" spans="1:22" ht="45">
       <c r="A20">
         <v>4</v>
       </c>
@@ -4446,7 +4450,7 @@
         <v>6</v>
       </c>
       <c r="N20" s="11" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="O20" s="4" t="s">
         <v>7</v>
@@ -4515,7 +4519,7 @@
         <v>4</v>
       </c>
       <c r="N21" s="11" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="O21" s="4" t="s">
         <v>43</v>
@@ -4542,7 +4546,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:22" ht="30">
+    <row r="22" spans="1:22" ht="45">
       <c r="A22">
         <v>5</v>
       </c>
@@ -4584,7 +4588,7 @@
         <v>6</v>
       </c>
       <c r="N22" s="11" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="O22" s="4" t="s">
         <v>12</v>
@@ -4653,7 +4657,7 @@
         <v>4</v>
       </c>
       <c r="N23" s="11" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="O23" s="4" t="s">
         <v>42</v>
@@ -5549,7 +5553,7 @@
         <v>1</v>
       </c>
       <c r="B44" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C44" t="s">
         <v>34</v>
@@ -5591,7 +5595,7 @@
         <v>2</v>
       </c>
       <c r="B45" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C45" t="s">
         <v>34</v>
@@ -5633,7 +5637,7 @@
         <v>3</v>
       </c>
       <c r="B46" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C46" t="s">
         <v>34</v>
@@ -5675,7 +5679,7 @@
         <v>4</v>
       </c>
       <c r="B47" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C47" t="s">
         <v>34</v>
@@ -5717,7 +5721,7 @@
         <v>5</v>
       </c>
       <c r="B48" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C48" t="s">
         <v>34</v>
@@ -8153,10 +8157,10 @@
         <v>0</v>
       </c>
       <c r="B106" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C106" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D106">
         <v>1</v>
@@ -8195,10 +8199,10 @@
         <v>1</v>
       </c>
       <c r="B107" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C107" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D107">
         <v>1</v>
@@ -8237,10 +8241,10 @@
         <v>2</v>
       </c>
       <c r="B108" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C108" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D108">
         <v>1</v>
@@ -8279,10 +8283,10 @@
         <v>3</v>
       </c>
       <c r="B109" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C109" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D109">
         <v>1</v>
@@ -8321,10 +8325,10 @@
         <v>4</v>
       </c>
       <c r="B110" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C110" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D110">
         <v>1</v>

</xml_diff>

<commit_message>
consistent spelling of \pilot
git-svn-id: file://localhost/tmp/svn2git/svn@7779 defb5e50-622e-49ec-a68e-d72c7db87b45
</commit_message>
<xml_diff>
--- a/papers/ccpe-cloud12/performance/pd.xlsx
+++ b/papers/ccpe-cloud12/performance/pd.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22416"/>
   <workbookPr showInkAnnotation="0" hidePivotFieldList="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1200" yWindow="0" windowWidth="48160" windowHeight="28300" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="26600" windowHeight="14920" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="1 CU" sheetId="1" r:id="rId1"/>
@@ -682,13 +682,7 @@
     <cellStyle name="Link" xfId="79" builtinId="8" hidden="1"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <numFmt numFmtId="164" formatCode="0.0"/>
     </dxf>
@@ -3091,7 +3085,7 @@
     <dataField name="Mittelwert - Order" fld="12" subtotal="average" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="1">
-    <format dxfId="2">
+    <format dxfId="0">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
   </formats>
@@ -3470,10 +3464,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V110"/>
+  <dimension ref="A1:W110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="N23" sqref="N23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="W22" sqref="W22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4201,7 +4195,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="17" spans="1:22" ht="45">
+    <row r="17" spans="1:23" ht="45">
       <c r="A17">
         <v>3</v>
       </c>
@@ -4270,7 +4264,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:22" ht="45">
+    <row r="18" spans="1:23" ht="45">
       <c r="A18">
         <v>3</v>
       </c>
@@ -4339,7 +4333,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:22" ht="45">
+    <row r="19" spans="1:23" ht="45">
       <c r="A19">
         <v>4</v>
       </c>
@@ -4408,7 +4402,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:22" ht="45">
+    <row r="20" spans="1:23" ht="45">
       <c r="A20">
         <v>4</v>
       </c>
@@ -4477,7 +4471,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:22" ht="45">
+    <row r="21" spans="1:23" ht="45">
       <c r="A21">
         <v>5</v>
       </c>
@@ -4545,8 +4539,12 @@
       <c r="V21" s="5">
         <v>5</v>
       </c>
-    </row>
-    <row r="22" spans="1:22" ht="45">
+      <c r="W21">
+        <f>Q21/Q20</f>
+        <v>4.9240667647029035</v>
+      </c>
+    </row>
+    <row r="22" spans="1:23" ht="45">
       <c r="A22">
         <v>5</v>
       </c>
@@ -4615,7 +4613,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:22" ht="45">
+    <row r="23" spans="1:23" ht="45">
       <c r="A23">
         <v>6</v>
       </c>
@@ -4683,8 +4681,12 @@
       <c r="V23" s="5">
         <v>7</v>
       </c>
-    </row>
-    <row r="24" spans="1:22">
+      <c r="W23">
+        <f>Q23/Q22</f>
+        <v>12.691792492071452</v>
+      </c>
+    </row>
+    <row r="24" spans="1:23">
       <c r="A24">
         <v>6</v>
       </c>
@@ -4750,7 +4752,7 @@
         <v>4.333333333333333</v>
       </c>
     </row>
-    <row r="25" spans="1:22">
+    <row r="25" spans="1:23">
       <c r="A25">
         <v>7</v>
       </c>
@@ -4792,7 +4794,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:22">
+    <row r="26" spans="1:23">
       <c r="A26">
         <v>7</v>
       </c>
@@ -4834,7 +4836,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:22">
+    <row r="27" spans="1:23">
       <c r="A27">
         <v>8</v>
       </c>
@@ -4876,7 +4878,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:22">
+    <row r="28" spans="1:23">
       <c r="A28">
         <v>8</v>
       </c>
@@ -4918,7 +4920,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="29" spans="1:22">
+    <row r="29" spans="1:23">
       <c r="A29">
         <v>9</v>
       </c>
@@ -4960,7 +4962,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:22">
+    <row r="30" spans="1:23">
       <c r="A30">
         <v>0</v>
       </c>
@@ -5002,7 +5004,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="1:22">
+    <row r="31" spans="1:23">
       <c r="A31">
         <v>1</v>
       </c>
@@ -5044,7 +5046,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="32" spans="1:22">
+    <row r="32" spans="1:23">
       <c r="A32">
         <v>2</v>
       </c>

</xml_diff>